<commit_message>
Updated db creation, values, and DD
</commit_message>
<xml_diff>
--- a/Group_1_DD_DD.xlsx
+++ b/Group_1_DD_DD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCTCC\Semester 3\Database Modeling 2\Doomsday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tard-\OneDrive\Desktop\School Assignments\CMSC 2201-23 DBII\Doomsday\DatabaseIIGroupOne-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DB7F62-4766-4ED7-8E3A-034F21BBD96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FBB03B-DD32-4099-A48F-5E097CE2F001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="12705" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="184">
   <si>
     <t>Database Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Starts with S</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Amount settlement has</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>How much the weapon costs</t>
   </si>
   <si>
-    <t>Food</t>
-  </si>
-  <si>
     <t>FoodDescription</t>
   </si>
   <si>
@@ -321,9 +315,6 @@
     <t>Starts with M</t>
   </si>
   <si>
-    <t>Check it starts with M and is integer</t>
-  </si>
-  <si>
     <t>MissionDate</t>
   </si>
   <si>
@@ -360,9 +351,6 @@
     <t>JobDescription</t>
   </si>
   <si>
-    <t>JobBasePay/Day</t>
-  </si>
-  <si>
     <t>The base pay for this job/day</t>
   </si>
   <si>
@@ -480,9 +468,6 @@
     <t>TransactionDetails</t>
   </si>
   <si>
-    <t>Transaction</t>
-  </si>
-  <si>
     <t>Unique ID for Transaction</t>
   </si>
   <si>
@@ -492,9 +477,6 @@
     <t>The type of housing that the settlement offers</t>
   </si>
   <si>
-    <t>Stored</t>
-  </si>
-  <si>
     <t>Location in settlement where to find weapons</t>
   </si>
   <si>
@@ -528,12 +510,6 @@
     <t>Location in settlement where to find items</t>
   </si>
   <si>
-    <t>Check it starts with MI</t>
-  </si>
-  <si>
-    <t>varchar(6)</t>
-  </si>
-  <si>
     <t>AmountOfMoney</t>
   </si>
   <si>
@@ -547,6 +523,69 @@
   </si>
   <si>
     <t>MiscPrice</t>
+  </si>
+  <si>
+    <t>Foods</t>
+  </si>
+  <si>
+    <t>WeaponQuantity</t>
+  </si>
+  <si>
+    <t>FoodStored</t>
+  </si>
+  <si>
+    <t>FoodQuantity</t>
+  </si>
+  <si>
+    <t>VehicleQuantity</t>
+  </si>
+  <si>
+    <t>MedicineStored</t>
+  </si>
+  <si>
+    <t>MedicineQuantity</t>
+  </si>
+  <si>
+    <t>MiscStored</t>
+  </si>
+  <si>
+    <t>MiscQuantity</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>QuantityBought</t>
+  </si>
+  <si>
+    <t>Check it starts with Q and is integer</t>
+  </si>
+  <si>
+    <t>JobBasePayPerDay</t>
+  </si>
+  <si>
+    <t>SetQuantity</t>
+  </si>
+  <si>
+    <t>Check it starts with U</t>
+  </si>
+  <si>
+    <t>WeaponStored</t>
+  </si>
+  <si>
+    <t>VehicleStored</t>
+  </si>
+  <si>
+    <t>PayPerPerson</t>
+  </si>
+  <si>
+    <t>Description of pay</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -735,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -996,6 +1035,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1277,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="B112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1858,7 @@
       </c>
       <c r="B2" s="5">
         <f ca="1">NOW()</f>
-        <v>44545.279090393517</v>
+        <v>44549.879600231485</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1926,10 +1968,10 @@
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="63"/>
       <c r="B8" s="63" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D8" s="63" t="s">
         <v>29</v>
@@ -1942,7 +1984,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I8" s="63"/>
       <c r="J8" s="63" t="s">
@@ -1952,10 +1994,10 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="82"/>
       <c r="B9" s="82" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C9" s="83" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D9" s="82" t="s">
         <v>18</v>
@@ -2027,7 +2069,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="72" t="s">
         <v>14</v>
@@ -2053,7 +2095,7 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="71"/>
       <c r="B14" s="71" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>34</v>
@@ -2077,7 +2119,7 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="71"/>
       <c r="B15" s="71" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C15" s="72" t="s">
         <v>35</v>
@@ -2101,7 +2143,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="71"/>
       <c r="B16" s="71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C16" s="72" t="s">
         <v>36</v>
@@ -2123,13 +2165,13 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="82"/>
       <c r="B17" s="82" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C17" s="83" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E17" s="83"/>
       <c r="F17" s="83"/>
@@ -2148,7 +2190,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
@@ -2196,10 +2238,10 @@
         <v>41</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>15</v>
@@ -2225,7 +2267,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" s="82" t="s">
         <v>15</v>
@@ -2250,7 +2292,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="92" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" s="93"/>
       <c r="D26" s="93"/>
@@ -2324,7 +2366,7 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
       <c r="B29" s="45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C29" s="46" t="s">
         <v>40</v>
@@ -2348,13 +2390,13 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
       <c r="B30" s="45" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
@@ -2385,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
@@ -2433,10 +2475,10 @@
         <v>41</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>15</v>
@@ -2489,7 +2531,7 @@
         <v>44</v>
       </c>
       <c r="D37" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -2508,7 +2550,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -2556,10 +2598,10 @@
         <v>13</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>15</v>
@@ -2572,7 +2614,7 @@
         <v>20</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I42" s="11"/>
       <c r="J42" s="82" t="s">
@@ -2582,10 +2624,10 @@
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="82"/>
       <c r="B43" s="82" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C43" s="83" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D43" s="82" t="s">
         <v>18</v>
@@ -2607,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -2681,10 +2723,10 @@
         <v>41</v>
       </c>
       <c r="B49" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>15</v>
@@ -2705,13 +2747,13 @@
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="82"/>
       <c r="B50" s="82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="83" t="s">
+      <c r="D50" s="82" t="s">
         <v>50</v>
-      </c>
-      <c r="D50" s="82" t="s">
-        <v>51</v>
       </c>
       <c r="E50" s="83"/>
       <c r="F50" s="83"/>
@@ -2742,7 +2784,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
@@ -2790,10 +2832,10 @@
         <v>13</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>15</v>
@@ -2804,7 +2846,7 @@
         <v>20</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I55" s="11"/>
       <c r="J55" s="11" t="s">
@@ -2814,10 +2856,10 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>18</v>
@@ -2836,13 +2878,13 @@
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
       <c r="B57" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
@@ -2858,10 +2900,10 @@
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="57"/>
       <c r="B58" s="57" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="C58" s="57" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D58" s="82" t="s">
         <v>18</v>
@@ -2880,13 +2922,13 @@
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="57"/>
       <c r="B59" s="57" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="C59" s="57" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D59" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E59" s="57"/>
       <c r="F59" s="57"/>
@@ -2916,7 +2958,7 @@
         <v>2</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
       <c r="C62" s="20"/>
       <c r="D62" s="20"/>
@@ -2964,10 +3006,10 @@
         <v>13</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>15</v>
@@ -2978,7 +3020,7 @@
         <v>20</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I64" s="11"/>
       <c r="J64" s="11" t="s">
@@ -2988,10 +3030,10 @@
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>18</v>
@@ -3010,13 +3052,13 @@
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D66" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E66" s="16"/>
       <c r="F66" s="16"/>
@@ -3032,10 +3074,10 @@
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="57"/>
       <c r="B67" s="57" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C67" s="57" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D67" s="82" t="s">
         <v>18</v>
@@ -3054,13 +3096,13 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="57"/>
       <c r="B68" s="57" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C68" s="57" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D68" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E68" s="57"/>
       <c r="F68" s="57"/>
@@ -3102,7 +3144,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C71" s="20"/>
       <c r="D71" s="20"/>
@@ -3150,10 +3192,10 @@
         <v>13</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C73" s="83" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>15</v>
@@ -3164,7 +3206,7 @@
         <v>20</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I73" s="11"/>
       <c r="J73" s="11" t="s">
@@ -3174,10 +3216,10 @@
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>18</v>
@@ -3196,13 +3238,13 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
       <c r="B75" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D75" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E75" s="16"/>
       <c r="F75" s="16"/>
@@ -3218,10 +3260,10 @@
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="57"/>
       <c r="B76" s="57" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="C76" s="57" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D76" s="82" t="s">
         <v>18</v>
@@ -3240,13 +3282,13 @@
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="57"/>
       <c r="B77" s="57" t="s">
-        <v>49</v>
+        <v>167</v>
       </c>
       <c r="C77" s="57" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D77" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E77" s="57"/>
       <c r="F77" s="57"/>
@@ -3265,7 +3307,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C80" s="20"/>
       <c r="D80" s="20"/>
@@ -3313,10 +3355,10 @@
         <v>13</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C82" s="83" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D82" s="11" t="s">
         <v>15</v>
@@ -3327,7 +3369,7 @@
         <v>20</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I82" s="11"/>
       <c r="J82" s="11" t="s">
@@ -3337,10 +3379,10 @@
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D83" s="11" t="s">
         <v>18</v>
@@ -3359,13 +3401,13 @@
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="16"/>
       <c r="B84" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D84" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
@@ -3381,10 +3423,10 @@
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="57"/>
       <c r="B85" s="57" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="C85" s="57" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D85" s="82" t="s">
         <v>18</v>
@@ -3403,13 +3445,13 @@
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="57"/>
       <c r="B86" s="57" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="C86" s="57" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D86" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E86" s="57"/>
       <c r="F86" s="57"/>
@@ -3428,7 +3470,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C89" s="20"/>
       <c r="D89" s="20"/>
@@ -3476,13 +3518,13 @@
         <v>13</v>
       </c>
       <c r="B91" s="91" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C91" s="83" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="E91" s="12"/>
       <c r="F91" s="13"/>
@@ -3490,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="I91" s="11"/>
       <c r="J91" s="11" t="s">
@@ -3500,10 +3542,10 @@
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
       <c r="B92" s="11" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>18</v>
@@ -3522,13 +3564,13 @@
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="16"/>
       <c r="B93" s="16" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D93" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E93" s="16"/>
       <c r="F93" s="16"/>
@@ -3544,10 +3586,10 @@
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="57"/>
       <c r="B94" s="57" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="C94" s="57" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D94" s="82" t="s">
         <v>18</v>
@@ -3566,13 +3608,13 @@
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="57"/>
       <c r="B95" s="57" t="s">
-        <v>49</v>
+        <v>171</v>
       </c>
       <c r="C95" s="57" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D95" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E95" s="57"/>
       <c r="F95" s="57"/>
@@ -3591,7 +3633,7 @@
         <v>2</v>
       </c>
       <c r="B98" s="58" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="C98" s="59"/>
       <c r="D98" s="59"/>
@@ -3639,23 +3681,23 @@
         <v>13</v>
       </c>
       <c r="B100" s="52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C100" s="53" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D100" s="82" t="s">
         <v>15</v>
       </c>
       <c r="E100" s="53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F100" s="54"/>
       <c r="G100" s="52" t="s">
         <v>20</v>
       </c>
       <c r="H100" s="52" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I100" s="52"/>
       <c r="J100" s="52" t="s">
@@ -3667,10 +3709,10 @@
         <v>21</v>
       </c>
       <c r="B101" s="52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C101" s="53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D101" s="52" t="s">
         <v>15</v>
@@ -3689,10 +3731,10 @@
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="57"/>
       <c r="B102" s="57" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C102" s="57" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D102" s="52" t="s">
         <v>37</v>
@@ -3711,13 +3753,13 @@
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="57"/>
       <c r="B103" s="57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C103" s="57" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D103" s="52" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E103" s="57"/>
       <c r="F103" s="57"/>
@@ -3736,7 +3778,7 @@
         <v>2</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C106" s="20"/>
       <c r="D106" s="20"/>
@@ -3784,10 +3826,10 @@
         <v>41</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D108" s="82" t="s">
         <v>15</v>
@@ -3808,10 +3850,10 @@
         <v>21</v>
       </c>
       <c r="B109" s="82" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C109" s="83" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D109" s="82" t="s">
         <v>15</v>
@@ -3824,7 +3866,7 @@
       <c r="H109" s="82"/>
       <c r="I109" s="82"/>
       <c r="J109" s="82" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
@@ -3832,10 +3874,10 @@
         <v>21</v>
       </c>
       <c r="B110" s="82" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C110" s="83" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D110" s="82" t="s">
         <v>15</v>
@@ -3848,7 +3890,7 @@
       <c r="H110" s="82"/>
       <c r="I110" s="82"/>
       <c r="J110" s="82" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
@@ -3856,10 +3898,10 @@
         <v>21</v>
       </c>
       <c r="B111" s="82" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C111" s="83" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D111" s="82" t="s">
         <v>15</v>
@@ -3872,7 +3914,7 @@
       <c r="H111" s="82"/>
       <c r="I111" s="82"/>
       <c r="J111" s="82" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -3880,10 +3922,10 @@
         <v>21</v>
       </c>
       <c r="B112" s="82" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C112" s="83" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D112" s="82" t="s">
         <v>15</v>
@@ -3896,7 +3938,7 @@
       <c r="H112" s="82"/>
       <c r="I112" s="82"/>
       <c r="J112" s="82" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -3904,10 +3946,10 @@
         <v>21</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>15</v>
@@ -3920,19 +3962,19 @@
       <c r="H113" s="11"/>
       <c r="I113" s="11"/>
       <c r="J113" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
       <c r="B114" s="16" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="C114" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E114" s="16"/>
       <c r="F114" s="16"/>
@@ -3951,7 +3993,7 @@
         <v>2</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C117" s="41"/>
       <c r="D117" s="41"/>
@@ -3999,23 +4041,23 @@
         <v>13</v>
       </c>
       <c r="B119" s="34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C119" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D119" s="82" t="s">
         <v>15</v>
       </c>
       <c r="E119" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F119" s="36"/>
       <c r="G119" s="34" t="s">
         <v>20</v>
       </c>
       <c r="H119" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I119" s="34"/>
       <c r="J119" s="34" t="s">
@@ -4025,10 +4067,10 @@
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="34"/>
       <c r="B120" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C120" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D120" s="34" t="s">
         <v>18</v>
@@ -4047,13 +4089,13 @@
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="39"/>
       <c r="B121" s="39" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C121" s="39" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D121" s="82" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E121" s="39"/>
       <c r="F121" s="39"/>
@@ -4072,7 +4114,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C124" s="30"/>
       <c r="D124" s="30"/>
@@ -4120,23 +4162,23 @@
         <v>13</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C126" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D126" s="82" t="s">
         <v>15</v>
       </c>
       <c r="E126" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F126" s="26"/>
       <c r="G126" s="24" t="s">
         <v>20</v>
       </c>
       <c r="H126" s="24" t="s">
-        <v>95</v>
+        <v>174</v>
       </c>
       <c r="I126" s="24"/>
       <c r="J126" s="24" t="s">
@@ -4146,10 +4188,10 @@
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="24"/>
       <c r="B127" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C127" s="25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D127" s="24" t="s">
         <v>37</v>
@@ -4168,10 +4210,10 @@
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="24"/>
       <c r="B128" s="24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C128" s="25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D128" s="24" t="s">
         <v>18</v>
@@ -4189,103 +4231,99 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="24" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B129" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C129" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D129" s="82" t="s">
         <v>15</v>
       </c>
       <c r="E129" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F129" s="26"/>
       <c r="G129" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H129" s="24" t="s">
-        <v>74</v>
-      </c>
+      <c r="H129" s="24"/>
       <c r="I129" s="24"/>
       <c r="J129" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="132" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="85" t="s">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="17"/>
+      <c r="B130" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C130" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="D130" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E130" s="90"/>
+      <c r="F130" s="95"/>
+      <c r="G130" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="H130" s="17"/>
+      <c r="I130" s="17"/>
+      <c r="J130" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B132" s="87" t="s">
-        <v>100</v>
-      </c>
-      <c r="C132" s="88"/>
-      <c r="D132" s="88"/>
-      <c r="E132" s="88"/>
-      <c r="F132" s="88"/>
-      <c r="G132" s="88"/>
-      <c r="H132" s="88"/>
-      <c r="I132" s="88"/>
-      <c r="J132" s="89"/>
-    </row>
-    <row r="133" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="86" t="s">
+      <c r="B133" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C133" s="88"/>
+      <c r="D133" s="88"/>
+      <c r="E133" s="88"/>
+      <c r="F133" s="88"/>
+      <c r="G133" s="88"/>
+      <c r="H133" s="88"/>
+      <c r="I133" s="88"/>
+      <c r="J133" s="89"/>
+    </row>
+    <row r="134" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B133" s="80" t="s">
+      <c r="B134" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C133" s="81" t="s">
+      <c r="C134" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="D133" s="81" t="s">
+      <c r="D134" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="81" t="s">
+      <c r="E134" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="F133" s="81" t="s">
+      <c r="F134" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="G133" s="81" t="s">
+      <c r="G134" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="H133" s="81" t="s">
+      <c r="H134" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="I133" s="81" t="s">
+      <c r="I134" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="J133" s="81" t="s">
+      <c r="J134" s="81" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="B134" s="82" t="s">
-        <v>80</v>
-      </c>
-      <c r="C134" s="83" t="s">
-        <v>103</v>
-      </c>
-      <c r="D134" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="E134" s="83"/>
-      <c r="F134" s="83"/>
-      <c r="G134" s="82" t="s">
-        <v>19</v>
-      </c>
-      <c r="H134" s="82"/>
-      <c r="I134" s="82"/>
-      <c r="J134" s="82" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -4293,22 +4331,46 @@
         <v>41</v>
       </c>
       <c r="B135" s="82" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C135" s="83" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D135" s="82" t="s">
         <v>15</v>
       </c>
       <c r="E135" s="83"/>
-      <c r="F135" s="84"/>
+      <c r="F135" s="83"/>
       <c r="G135" s="82" t="s">
         <v>19</v>
       </c>
       <c r="H135" s="82"/>
       <c r="I135" s="82"/>
       <c r="J135" s="82" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B136" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="C136" s="83" t="s">
+        <v>99</v>
+      </c>
+      <c r="D136" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="E136" s="83"/>
+      <c r="F136" s="84"/>
+      <c r="G136" s="82" t="s">
+        <v>19</v>
+      </c>
+      <c r="H136" s="82"/>
+      <c r="I136" s="82"/>
+      <c r="J136" s="82" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4318,31 +4380,16 @@
     <mergeCell ref="B4:J4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65504:F65519 WVO983007:WVP983022 WLS983007:WLT983022 WBW983007:WBX983022 VSA983007:VSB983022 VIE983007:VIF983022 UYI983007:UYJ983022 UOM983007:UON983022 UEQ983007:UER983022 TUU983007:TUV983022 TKY983007:TKZ983022 TBC983007:TBD983022 SRG983007:SRH983022 SHK983007:SHL983022 RXO983007:RXP983022 RNS983007:RNT983022 RDW983007:RDX983022 QUA983007:QUB983022 QKE983007:QKF983022 QAI983007:QAJ983022 PQM983007:PQN983022 PGQ983007:PGR983022 OWU983007:OWV983022 OMY983007:OMZ983022 ODC983007:ODD983022 NTG983007:NTH983022 NJK983007:NJL983022 MZO983007:MZP983022 MPS983007:MPT983022 MFW983007:MFX983022 LWA983007:LWB983022 LME983007:LMF983022 LCI983007:LCJ983022 KSM983007:KSN983022 KIQ983007:KIR983022 JYU983007:JYV983022 JOY983007:JOZ983022 JFC983007:JFD983022 IVG983007:IVH983022 ILK983007:ILL983022 IBO983007:IBP983022 HRS983007:HRT983022 HHW983007:HHX983022 GYA983007:GYB983022 GOE983007:GOF983022 GEI983007:GEJ983022 FUM983007:FUN983022 FKQ983007:FKR983022 FAU983007:FAV983022 EQY983007:EQZ983022 EHC983007:EHD983022 DXG983007:DXH983022 DNK983007:DNL983022 DDO983007:DDP983022 CTS983007:CTT983022 CJW983007:CJX983022 CAA983007:CAB983022 BQE983007:BQF983022 BGI983007:BGJ983022 AWM983007:AWN983022 AMQ983007:AMR983022 ACU983007:ACV983022 SY983007:SZ983022 JC983007:JD983022 F983008:F983023 WVO917471:WVP917486 WLS917471:WLT917486 WBW917471:WBX917486 VSA917471:VSB917486 VIE917471:VIF917486 UYI917471:UYJ917486 UOM917471:UON917486 UEQ917471:UER917486 TUU917471:TUV917486 TKY917471:TKZ917486 TBC917471:TBD917486 SRG917471:SRH917486 SHK917471:SHL917486 RXO917471:RXP917486 RNS917471:RNT917486 RDW917471:RDX917486 QUA917471:QUB917486 QKE917471:QKF917486 QAI917471:QAJ917486 PQM917471:PQN917486 PGQ917471:PGR917486 OWU917471:OWV917486 OMY917471:OMZ917486 ODC917471:ODD917486 NTG917471:NTH917486 NJK917471:NJL917486 MZO917471:MZP917486 MPS917471:MPT917486 MFW917471:MFX917486 LWA917471:LWB917486 LME917471:LMF917486 LCI917471:LCJ917486 KSM917471:KSN917486 KIQ917471:KIR917486 JYU917471:JYV917486 JOY917471:JOZ917486 JFC917471:JFD917486 IVG917471:IVH917486 ILK917471:ILL917486 IBO917471:IBP917486 HRS917471:HRT917486 HHW917471:HHX917486 GYA917471:GYB917486 GOE917471:GOF917486 GEI917471:GEJ917486 FUM917471:FUN917486 FKQ917471:FKR917486 FAU917471:FAV917486 EQY917471:EQZ917486 EHC917471:EHD917486 DXG917471:DXH917486 DNK917471:DNL917486 DDO917471:DDP917486 CTS917471:CTT917486 CJW917471:CJX917486 CAA917471:CAB917486 BQE917471:BQF917486 BGI917471:BGJ917486 AWM917471:AWN917486 AMQ917471:AMR917486 ACU917471:ACV917486 SY917471:SZ917486 JC917471:JD917486 F917472:F917487 WVO851935:WVP851950 WLS851935:WLT851950 WBW851935:WBX851950 VSA851935:VSB851950 VIE851935:VIF851950 UYI851935:UYJ851950 UOM851935:UON851950 UEQ851935:UER851950 TUU851935:TUV851950 TKY851935:TKZ851950 TBC851935:TBD851950 SRG851935:SRH851950 SHK851935:SHL851950 RXO851935:RXP851950 RNS851935:RNT851950 RDW851935:RDX851950 QUA851935:QUB851950 QKE851935:QKF851950 QAI851935:QAJ851950 PQM851935:PQN851950 PGQ851935:PGR851950 OWU851935:OWV851950 OMY851935:OMZ851950 ODC851935:ODD851950 NTG851935:NTH851950 NJK851935:NJL851950 MZO851935:MZP851950 MPS851935:MPT851950 MFW851935:MFX851950 LWA851935:LWB851950 LME851935:LMF851950 LCI851935:LCJ851950 KSM851935:KSN851950 KIQ851935:KIR851950 JYU851935:JYV851950 JOY851935:JOZ851950 JFC851935:JFD851950 IVG851935:IVH851950 ILK851935:ILL851950 IBO851935:IBP851950 HRS851935:HRT851950 HHW851935:HHX851950 GYA851935:GYB851950 GOE851935:GOF851950 GEI851935:GEJ851950 FUM851935:FUN851950 FKQ851935:FKR851950 FAU851935:FAV851950 EQY851935:EQZ851950 EHC851935:EHD851950 DXG851935:DXH851950 DNK851935:DNL851950 DDO851935:DDP851950 CTS851935:CTT851950 CJW851935:CJX851950 CAA851935:CAB851950 BQE851935:BQF851950 BGI851935:BGJ851950 AWM851935:AWN851950 AMQ851935:AMR851950 ACU851935:ACV851950 SY851935:SZ851950 JC851935:JD851950 F851936:F851951 WVO786399:WVP786414 WLS786399:WLT786414 WBW786399:WBX786414 VSA786399:VSB786414 VIE786399:VIF786414 UYI786399:UYJ786414 UOM786399:UON786414 UEQ786399:UER786414 TUU786399:TUV786414 TKY786399:TKZ786414 TBC786399:TBD786414 SRG786399:SRH786414 SHK786399:SHL786414 RXO786399:RXP786414 RNS786399:RNT786414 RDW786399:RDX786414 QUA786399:QUB786414 QKE786399:QKF786414 QAI786399:QAJ786414 PQM786399:PQN786414 PGQ786399:PGR786414 OWU786399:OWV786414 OMY786399:OMZ786414 ODC786399:ODD786414 NTG786399:NTH786414 NJK786399:NJL786414 MZO786399:MZP786414 MPS786399:MPT786414 MFW786399:MFX786414 LWA786399:LWB786414 LME786399:LMF786414 LCI786399:LCJ786414 KSM786399:KSN786414 KIQ786399:KIR786414 JYU786399:JYV786414 JOY786399:JOZ786414 JFC786399:JFD786414 IVG786399:IVH786414 ILK786399:ILL786414 IBO786399:IBP786414 HRS786399:HRT786414 HHW786399:HHX786414 GYA786399:GYB786414 GOE786399:GOF786414 GEI786399:GEJ786414 FUM786399:FUN786414 FKQ786399:FKR786414 FAU786399:FAV786414 EQY786399:EQZ786414 EHC786399:EHD786414 DXG786399:DXH786414 DNK786399:DNL786414 DDO786399:DDP786414 CTS786399:CTT786414 CJW786399:CJX786414 CAA786399:CAB786414 BQE786399:BQF786414 BGI786399:BGJ786414 AWM786399:AWN786414 AMQ786399:AMR786414 ACU786399:ACV786414 SY786399:SZ786414 JC786399:JD786414 F786400:F786415 WVO720863:WVP720878 WLS720863:WLT720878 WBW720863:WBX720878 VSA720863:VSB720878 VIE720863:VIF720878 UYI720863:UYJ720878 UOM720863:UON720878 UEQ720863:UER720878 TUU720863:TUV720878 TKY720863:TKZ720878 TBC720863:TBD720878 SRG720863:SRH720878 SHK720863:SHL720878 RXO720863:RXP720878 RNS720863:RNT720878 RDW720863:RDX720878 QUA720863:QUB720878 QKE720863:QKF720878 QAI720863:QAJ720878 PQM720863:PQN720878 PGQ720863:PGR720878 OWU720863:OWV720878 OMY720863:OMZ720878 ODC720863:ODD720878 NTG720863:NTH720878 NJK720863:NJL720878 MZO720863:MZP720878 MPS720863:MPT720878 MFW720863:MFX720878 LWA720863:LWB720878 LME720863:LMF720878 LCI720863:LCJ720878 KSM720863:KSN720878 KIQ720863:KIR720878 JYU720863:JYV720878 JOY720863:JOZ720878 JFC720863:JFD720878 IVG720863:IVH720878 ILK720863:ILL720878 IBO720863:IBP720878 HRS720863:HRT720878 HHW720863:HHX720878 GYA720863:GYB720878 GOE720863:GOF720878 GEI720863:GEJ720878 FUM720863:FUN720878 FKQ720863:FKR720878 FAU720863:FAV720878 EQY720863:EQZ720878 EHC720863:EHD720878 DXG720863:DXH720878 DNK720863:DNL720878 DDO720863:DDP720878 CTS720863:CTT720878 CJW720863:CJX720878 CAA720863:CAB720878 BQE720863:BQF720878 BGI720863:BGJ720878 AWM720863:AWN720878 AMQ720863:AMR720878 ACU720863:ACV720878 SY720863:SZ720878 JC720863:JD720878 F720864:F720879 WVO655327:WVP655342 WLS655327:WLT655342 WBW655327:WBX655342 VSA655327:VSB655342 VIE655327:VIF655342 UYI655327:UYJ655342 UOM655327:UON655342 UEQ655327:UER655342 TUU655327:TUV655342 TKY655327:TKZ655342 TBC655327:TBD655342 SRG655327:SRH655342 SHK655327:SHL655342 RXO655327:RXP655342 RNS655327:RNT655342 RDW655327:RDX655342 QUA655327:QUB655342 QKE655327:QKF655342 QAI655327:QAJ655342 PQM655327:PQN655342 PGQ655327:PGR655342 OWU655327:OWV655342 OMY655327:OMZ655342 ODC655327:ODD655342 NTG655327:NTH655342 NJK655327:NJL655342 MZO655327:MZP655342 MPS655327:MPT655342 MFW655327:MFX655342 LWA655327:LWB655342 LME655327:LMF655342 LCI655327:LCJ655342 KSM655327:KSN655342 KIQ655327:KIR655342 JYU655327:JYV655342 JOY655327:JOZ655342 JFC655327:JFD655342 IVG655327:IVH655342 ILK655327:ILL655342 IBO655327:IBP655342 HRS655327:HRT655342 HHW655327:HHX655342 GYA655327:GYB655342 GOE655327:GOF655342 GEI655327:GEJ655342 FUM655327:FUN655342 FKQ655327:FKR655342 FAU655327:FAV655342 EQY655327:EQZ655342 EHC655327:EHD655342 DXG655327:DXH655342 DNK655327:DNL655342 DDO655327:DDP655342 CTS655327:CTT655342 CJW655327:CJX655342 CAA655327:CAB655342 BQE655327:BQF655342 BGI655327:BGJ655342 AWM655327:AWN655342 AMQ655327:AMR655342 ACU655327:ACV655342 SY655327:SZ655342 JC655327:JD655342 F655328:F655343 WVO589791:WVP589806 WLS589791:WLT589806 WBW589791:WBX589806 VSA589791:VSB589806 VIE589791:VIF589806 UYI589791:UYJ589806 UOM589791:UON589806 UEQ589791:UER589806 TUU589791:TUV589806 TKY589791:TKZ589806 TBC589791:TBD589806 SRG589791:SRH589806 SHK589791:SHL589806 RXO589791:RXP589806 RNS589791:RNT589806 RDW589791:RDX589806 QUA589791:QUB589806 QKE589791:QKF589806 QAI589791:QAJ589806 PQM589791:PQN589806 PGQ589791:PGR589806 OWU589791:OWV589806 OMY589791:OMZ589806 ODC589791:ODD589806 NTG589791:NTH589806 NJK589791:NJL589806 MZO589791:MZP589806 MPS589791:MPT589806 MFW589791:MFX589806 LWA589791:LWB589806 LME589791:LMF589806 LCI589791:LCJ589806 KSM589791:KSN589806 KIQ589791:KIR589806 JYU589791:JYV589806 JOY589791:JOZ589806 JFC589791:JFD589806 IVG589791:IVH589806 ILK589791:ILL589806 IBO589791:IBP589806 HRS589791:HRT589806 HHW589791:HHX589806 GYA589791:GYB589806 GOE589791:GOF589806 GEI589791:GEJ589806 FUM589791:FUN589806 FKQ589791:FKR589806 FAU589791:FAV589806 EQY589791:EQZ589806 EHC589791:EHD589806 DXG589791:DXH589806 DNK589791:DNL589806 DDO589791:DDP589806 CTS589791:CTT589806 CJW589791:CJX589806 CAA589791:CAB589806 BQE589791:BQF589806 BGI589791:BGJ589806 AWM589791:AWN589806 AMQ589791:AMR589806 ACU589791:ACV589806 SY589791:SZ589806 JC589791:JD589806 F589792:F589807 WVO524255:WVP524270 WLS524255:WLT524270 WBW524255:WBX524270 VSA524255:VSB524270 VIE524255:VIF524270 UYI524255:UYJ524270 UOM524255:UON524270 UEQ524255:UER524270 TUU524255:TUV524270 TKY524255:TKZ524270 TBC524255:TBD524270 SRG524255:SRH524270 SHK524255:SHL524270 RXO524255:RXP524270 RNS524255:RNT524270 RDW524255:RDX524270 QUA524255:QUB524270 QKE524255:QKF524270 QAI524255:QAJ524270 PQM524255:PQN524270 PGQ524255:PGR524270 OWU524255:OWV524270 OMY524255:OMZ524270 ODC524255:ODD524270 NTG524255:NTH524270 NJK524255:NJL524270 MZO524255:MZP524270 MPS524255:MPT524270 MFW524255:MFX524270 LWA524255:LWB524270 LME524255:LMF524270 LCI524255:LCJ524270 KSM524255:KSN524270 KIQ524255:KIR524270 JYU524255:JYV524270 JOY524255:JOZ524270 JFC524255:JFD524270 IVG524255:IVH524270 ILK524255:ILL524270 IBO524255:IBP524270 HRS524255:HRT524270 HHW524255:HHX524270 GYA524255:GYB524270 GOE524255:GOF524270 GEI524255:GEJ524270 FUM524255:FUN524270 FKQ524255:FKR524270 FAU524255:FAV524270 EQY524255:EQZ524270 EHC524255:EHD524270 DXG524255:DXH524270 DNK524255:DNL524270 DDO524255:DDP524270 CTS524255:CTT524270 CJW524255:CJX524270 CAA524255:CAB524270 BQE524255:BQF524270 BGI524255:BGJ524270 AWM524255:AWN524270 AMQ524255:AMR524270 ACU524255:ACV524270 SY524255:SZ524270 JC524255:JD524270 F524256:F524271 WVO458719:WVP458734 WLS458719:WLT458734 WBW458719:WBX458734 VSA458719:VSB458734 VIE458719:VIF458734 UYI458719:UYJ458734 UOM458719:UON458734 UEQ458719:UER458734 TUU458719:TUV458734 TKY458719:TKZ458734 TBC458719:TBD458734 SRG458719:SRH458734 SHK458719:SHL458734 RXO458719:RXP458734 RNS458719:RNT458734 RDW458719:RDX458734 QUA458719:QUB458734 QKE458719:QKF458734 QAI458719:QAJ458734 PQM458719:PQN458734 PGQ458719:PGR458734 OWU458719:OWV458734 OMY458719:OMZ458734 ODC458719:ODD458734 NTG458719:NTH458734 NJK458719:NJL458734 MZO458719:MZP458734 MPS458719:MPT458734 MFW458719:MFX458734 LWA458719:LWB458734 LME458719:LMF458734 LCI458719:LCJ458734 KSM458719:KSN458734 KIQ458719:KIR458734 JYU458719:JYV458734 JOY458719:JOZ458734 JFC458719:JFD458734 IVG458719:IVH458734 ILK458719:ILL458734 IBO458719:IBP458734 HRS458719:HRT458734 HHW458719:HHX458734 GYA458719:GYB458734 GOE458719:GOF458734 GEI458719:GEJ458734 FUM458719:FUN458734 FKQ458719:FKR458734 FAU458719:FAV458734 EQY458719:EQZ458734 EHC458719:EHD458734 DXG458719:DXH458734 DNK458719:DNL458734 DDO458719:DDP458734 CTS458719:CTT458734 CJW458719:CJX458734 CAA458719:CAB458734 BQE458719:BQF458734 BGI458719:BGJ458734 AWM458719:AWN458734 AMQ458719:AMR458734 ACU458719:ACV458734 SY458719:SZ458734 JC458719:JD458734 F458720:F458735 WVO393183:WVP393198 WLS393183:WLT393198 WBW393183:WBX393198 VSA393183:VSB393198 VIE393183:VIF393198 UYI393183:UYJ393198 UOM393183:UON393198 UEQ393183:UER393198 TUU393183:TUV393198 TKY393183:TKZ393198 TBC393183:TBD393198 SRG393183:SRH393198 SHK393183:SHL393198 RXO393183:RXP393198 RNS393183:RNT393198 RDW393183:RDX393198 QUA393183:QUB393198 QKE393183:QKF393198 QAI393183:QAJ393198 PQM393183:PQN393198 PGQ393183:PGR393198 OWU393183:OWV393198 OMY393183:OMZ393198 ODC393183:ODD393198 NTG393183:NTH393198 NJK393183:NJL393198 MZO393183:MZP393198 MPS393183:MPT393198 MFW393183:MFX393198 LWA393183:LWB393198 LME393183:LMF393198 LCI393183:LCJ393198 KSM393183:KSN393198 KIQ393183:KIR393198 JYU393183:JYV393198 JOY393183:JOZ393198 JFC393183:JFD393198 IVG393183:IVH393198 ILK393183:ILL393198 IBO393183:IBP393198 HRS393183:HRT393198 HHW393183:HHX393198 GYA393183:GYB393198 GOE393183:GOF393198 GEI393183:GEJ393198 FUM393183:FUN393198 FKQ393183:FKR393198 FAU393183:FAV393198 EQY393183:EQZ393198 EHC393183:EHD393198 DXG393183:DXH393198 DNK393183:DNL393198 DDO393183:DDP393198 CTS393183:CTT393198 CJW393183:CJX393198 CAA393183:CAB393198 BQE393183:BQF393198 BGI393183:BGJ393198 AWM393183:AWN393198 AMQ393183:AMR393198 ACU393183:ACV393198 SY393183:SZ393198 JC393183:JD393198 F393184:F393199 WVO327647:WVP327662 WLS327647:WLT327662 WBW327647:WBX327662 VSA327647:VSB327662 VIE327647:VIF327662 UYI327647:UYJ327662 UOM327647:UON327662 UEQ327647:UER327662 TUU327647:TUV327662 TKY327647:TKZ327662 TBC327647:TBD327662 SRG327647:SRH327662 SHK327647:SHL327662 RXO327647:RXP327662 RNS327647:RNT327662 RDW327647:RDX327662 QUA327647:QUB327662 QKE327647:QKF327662 QAI327647:QAJ327662 PQM327647:PQN327662 PGQ327647:PGR327662 OWU327647:OWV327662 OMY327647:OMZ327662 ODC327647:ODD327662 NTG327647:NTH327662 NJK327647:NJL327662 MZO327647:MZP327662 MPS327647:MPT327662 MFW327647:MFX327662 LWA327647:LWB327662 LME327647:LMF327662 LCI327647:LCJ327662 KSM327647:KSN327662 KIQ327647:KIR327662 JYU327647:JYV327662 JOY327647:JOZ327662 JFC327647:JFD327662 IVG327647:IVH327662 ILK327647:ILL327662 IBO327647:IBP327662 HRS327647:HRT327662 HHW327647:HHX327662 GYA327647:GYB327662 GOE327647:GOF327662 GEI327647:GEJ327662 FUM327647:FUN327662 FKQ327647:FKR327662 FAU327647:FAV327662 EQY327647:EQZ327662 EHC327647:EHD327662 DXG327647:DXH327662 DNK327647:DNL327662 DDO327647:DDP327662 CTS327647:CTT327662 CJW327647:CJX327662 CAA327647:CAB327662 BQE327647:BQF327662 BGI327647:BGJ327662 AWM327647:AWN327662 AMQ327647:AMR327662 ACU327647:ACV327662 SY327647:SZ327662 JC327647:JD327662 F327648:F327663 WVO262111:WVP262126 WLS262111:WLT262126 WBW262111:WBX262126 VSA262111:VSB262126 VIE262111:VIF262126 UYI262111:UYJ262126 UOM262111:UON262126 UEQ262111:UER262126 TUU262111:TUV262126 TKY262111:TKZ262126 TBC262111:TBD262126 SRG262111:SRH262126 SHK262111:SHL262126 RXO262111:RXP262126 RNS262111:RNT262126 RDW262111:RDX262126 QUA262111:QUB262126 QKE262111:QKF262126 QAI262111:QAJ262126 PQM262111:PQN262126 PGQ262111:PGR262126 OWU262111:OWV262126 OMY262111:OMZ262126 ODC262111:ODD262126 NTG262111:NTH262126 NJK262111:NJL262126 MZO262111:MZP262126 MPS262111:MPT262126 MFW262111:MFX262126 LWA262111:LWB262126 LME262111:LMF262126 LCI262111:LCJ262126 KSM262111:KSN262126 KIQ262111:KIR262126 JYU262111:JYV262126 JOY262111:JOZ262126 JFC262111:JFD262126 IVG262111:IVH262126 ILK262111:ILL262126 IBO262111:IBP262126 HRS262111:HRT262126 HHW262111:HHX262126 GYA262111:GYB262126 GOE262111:GOF262126 GEI262111:GEJ262126 FUM262111:FUN262126 FKQ262111:FKR262126 FAU262111:FAV262126 EQY262111:EQZ262126 EHC262111:EHD262126 DXG262111:DXH262126 DNK262111:DNL262126 DDO262111:DDP262126 CTS262111:CTT262126 CJW262111:CJX262126 CAA262111:CAB262126 BQE262111:BQF262126 BGI262111:BGJ262126 AWM262111:AWN262126 AMQ262111:AMR262126 ACU262111:ACV262126 SY262111:SZ262126 JC262111:JD262126 F262112:F262127 WVO196575:WVP196590 WLS196575:WLT196590 WBW196575:WBX196590 VSA196575:VSB196590 VIE196575:VIF196590 UYI196575:UYJ196590 UOM196575:UON196590 UEQ196575:UER196590 TUU196575:TUV196590 TKY196575:TKZ196590 TBC196575:TBD196590 SRG196575:SRH196590 SHK196575:SHL196590 RXO196575:RXP196590 RNS196575:RNT196590 RDW196575:RDX196590 QUA196575:QUB196590 QKE196575:QKF196590 QAI196575:QAJ196590 PQM196575:PQN196590 PGQ196575:PGR196590 OWU196575:OWV196590 OMY196575:OMZ196590 ODC196575:ODD196590 NTG196575:NTH196590 NJK196575:NJL196590 MZO196575:MZP196590 MPS196575:MPT196590 MFW196575:MFX196590 LWA196575:LWB196590 LME196575:LMF196590 LCI196575:LCJ196590 KSM196575:KSN196590 KIQ196575:KIR196590 JYU196575:JYV196590 JOY196575:JOZ196590 JFC196575:JFD196590 IVG196575:IVH196590 ILK196575:ILL196590 IBO196575:IBP196590 HRS196575:HRT196590 HHW196575:HHX196590 GYA196575:GYB196590 GOE196575:GOF196590 GEI196575:GEJ196590 FUM196575:FUN196590 FKQ196575:FKR196590 FAU196575:FAV196590 EQY196575:EQZ196590 EHC196575:EHD196590 DXG196575:DXH196590 DNK196575:DNL196590 DDO196575:DDP196590 CTS196575:CTT196590 CJW196575:CJX196590 CAA196575:CAB196590 BQE196575:BQF196590 BGI196575:BGJ196590 AWM196575:AWN196590 AMQ196575:AMR196590 ACU196575:ACV196590 SY196575:SZ196590 JC196575:JD196590 F196576:F196591 WVO131039:WVP131054 WLS131039:WLT131054 WBW131039:WBX131054 VSA131039:VSB131054 VIE131039:VIF131054 UYI131039:UYJ131054 UOM131039:UON131054 UEQ131039:UER131054 TUU131039:TUV131054 TKY131039:TKZ131054 TBC131039:TBD131054 SRG131039:SRH131054 SHK131039:SHL131054 RXO131039:RXP131054 RNS131039:RNT131054 RDW131039:RDX131054 QUA131039:QUB131054 QKE131039:QKF131054 QAI131039:QAJ131054 PQM131039:PQN131054 PGQ131039:PGR131054 OWU131039:OWV131054 OMY131039:OMZ131054 ODC131039:ODD131054 NTG131039:NTH131054 NJK131039:NJL131054 MZO131039:MZP131054 MPS131039:MPT131054 MFW131039:MFX131054 LWA131039:LWB131054 LME131039:LMF131054 LCI131039:LCJ131054 KSM131039:KSN131054 KIQ131039:KIR131054 JYU131039:JYV131054 JOY131039:JOZ131054 JFC131039:JFD131054 IVG131039:IVH131054 ILK131039:ILL131054 IBO131039:IBP131054 HRS131039:HRT131054 HHW131039:HHX131054 GYA131039:GYB131054 GOE131039:GOF131054 GEI131039:GEJ131054 FUM131039:FUN131054 FKQ131039:FKR131054 FAU131039:FAV131054 EQY131039:EQZ131054 EHC131039:EHD131054 DXG131039:DXH131054 DNK131039:DNL131054 DDO131039:DDP131054 CTS131039:CTT131054 CJW131039:CJX131054 CAA131039:CAB131054 BQE131039:BQF131054 BGI131039:BGJ131054 AWM131039:AWN131054 AMQ131039:AMR131054 ACU131039:ACV131054 SY131039:SZ131054 JC131039:JD131054 F131040:F131055 WVO65503:WVP65518 WLS65503:WLT65518 WBW65503:WBX65518 VSA65503:VSB65518 VIE65503:VIF65518 UYI65503:UYJ65518 UOM65503:UON65518 UEQ65503:UER65518 TUU65503:TUV65518 TKY65503:TKZ65518 TBC65503:TBD65518 SRG65503:SRH65518 SHK65503:SHL65518 RXO65503:RXP65518 RNS65503:RNT65518 RDW65503:RDX65518 QUA65503:QUB65518 QKE65503:QKF65518 QAI65503:QAJ65518 PQM65503:PQN65518 PGQ65503:PGR65518 OWU65503:OWV65518 OMY65503:OMZ65518 ODC65503:ODD65518 NTG65503:NTH65518 NJK65503:NJL65518 MZO65503:MZP65518 MPS65503:MPT65518 MFW65503:MFX65518 LWA65503:LWB65518 LME65503:LMF65518 LCI65503:LCJ65518 KSM65503:KSN65518 KIQ65503:KIR65518 JYU65503:JYV65518 JOY65503:JOZ65518 JFC65503:JFD65518 IVG65503:IVH65518 ILK65503:ILL65518 IBO65503:IBP65518 HRS65503:HRT65518 HHW65503:HHX65518 GYA65503:GYB65518 GOE65503:GOF65518 GEI65503:GEJ65518 FUM65503:FUN65518 FKQ65503:FKR65518 FAU65503:FAV65518 EQY65503:EQZ65518 EHC65503:EHD65518 DXG65503:DXH65518 DNK65503:DNL65518 DDO65503:DDP65518 CTS65503:CTT65518 CJW65503:CJX65518 CAA65503:CAB65518 BQE65503:BQF65518 BGI65503:BGJ65518 AWM65503:AWN65518 AMQ65503:AMR65518 ACU65503:ACV65518 SY65503:SZ65518 JC65503:JD65518 WLI14:WLJ17 WBM14:WBN17 VRQ14:VRR17 VHU14:VHV17 UXY14:UXZ17 UOC14:UOD17 UEG14:UEH17 TUK14:TUL17 TKO14:TKP17 TAS14:TAT17 SQW14:SQX17 SHA14:SHB17 RXE14:RXF17 RNI14:RNJ17 RDM14:RDN17 QTQ14:QTR17 QJU14:QJV17 PZY14:PZZ17 PQC14:PQD17 PGG14:PGH17 OWK14:OWL17 OMO14:OMP17 OCS14:OCT17 NSW14:NSX17 NJA14:NJB17 MZE14:MZF17 MPI14:MPJ17 MFM14:MFN17 LVQ14:LVR17 LLU14:LLV17 LBY14:LBZ17 KSC14:KSD17 KIG14:KIH17 JYK14:JYL17 JOO14:JOP17 JES14:JET17 IUW14:IUX17 ILA14:ILB17 IBE14:IBF17 HRI14:HRJ17 HHM14:HHN17 GXQ14:GXR17 GNU14:GNV17 GDY14:GDZ17 FUC14:FUD17 FKG14:FKH17 FAK14:FAL17 EQO14:EQP17 EGS14:EGT17 DWW14:DWX17 DNA14:DNB17 DDE14:DDF17 CTI14:CTJ17 CJM14:CJN17 BZQ14:BZR17 BPU14:BPV17 BFY14:BFZ17 AWC14:AWD17 AMG14:AMH17 ACK14:ACL17 SO14:SP17 IS14:IT17 WVE14:WVF17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65505:F65520 WVO983008:WVP983023 WLS983008:WLT983023 WBW983008:WBX983023 VSA983008:VSB983023 VIE983008:VIF983023 UYI983008:UYJ983023 UOM983008:UON983023 UEQ983008:UER983023 TUU983008:TUV983023 TKY983008:TKZ983023 TBC983008:TBD983023 SRG983008:SRH983023 SHK983008:SHL983023 RXO983008:RXP983023 RNS983008:RNT983023 RDW983008:RDX983023 QUA983008:QUB983023 QKE983008:QKF983023 QAI983008:QAJ983023 PQM983008:PQN983023 PGQ983008:PGR983023 OWU983008:OWV983023 OMY983008:OMZ983023 ODC983008:ODD983023 NTG983008:NTH983023 NJK983008:NJL983023 MZO983008:MZP983023 MPS983008:MPT983023 MFW983008:MFX983023 LWA983008:LWB983023 LME983008:LMF983023 LCI983008:LCJ983023 KSM983008:KSN983023 KIQ983008:KIR983023 JYU983008:JYV983023 JOY983008:JOZ983023 JFC983008:JFD983023 IVG983008:IVH983023 ILK983008:ILL983023 IBO983008:IBP983023 HRS983008:HRT983023 HHW983008:HHX983023 GYA983008:GYB983023 GOE983008:GOF983023 GEI983008:GEJ983023 FUM983008:FUN983023 FKQ983008:FKR983023 FAU983008:FAV983023 EQY983008:EQZ983023 EHC983008:EHD983023 DXG983008:DXH983023 DNK983008:DNL983023 DDO983008:DDP983023 CTS983008:CTT983023 CJW983008:CJX983023 CAA983008:CAB983023 BQE983008:BQF983023 BGI983008:BGJ983023 AWM983008:AWN983023 AMQ983008:AMR983023 ACU983008:ACV983023 SY983008:SZ983023 JC983008:JD983023 F983009:F983024 WVO917472:WVP917487 WLS917472:WLT917487 WBW917472:WBX917487 VSA917472:VSB917487 VIE917472:VIF917487 UYI917472:UYJ917487 UOM917472:UON917487 UEQ917472:UER917487 TUU917472:TUV917487 TKY917472:TKZ917487 TBC917472:TBD917487 SRG917472:SRH917487 SHK917472:SHL917487 RXO917472:RXP917487 RNS917472:RNT917487 RDW917472:RDX917487 QUA917472:QUB917487 QKE917472:QKF917487 QAI917472:QAJ917487 PQM917472:PQN917487 PGQ917472:PGR917487 OWU917472:OWV917487 OMY917472:OMZ917487 ODC917472:ODD917487 NTG917472:NTH917487 NJK917472:NJL917487 MZO917472:MZP917487 MPS917472:MPT917487 MFW917472:MFX917487 LWA917472:LWB917487 LME917472:LMF917487 LCI917472:LCJ917487 KSM917472:KSN917487 KIQ917472:KIR917487 JYU917472:JYV917487 JOY917472:JOZ917487 JFC917472:JFD917487 IVG917472:IVH917487 ILK917472:ILL917487 IBO917472:IBP917487 HRS917472:HRT917487 HHW917472:HHX917487 GYA917472:GYB917487 GOE917472:GOF917487 GEI917472:GEJ917487 FUM917472:FUN917487 FKQ917472:FKR917487 FAU917472:FAV917487 EQY917472:EQZ917487 EHC917472:EHD917487 DXG917472:DXH917487 DNK917472:DNL917487 DDO917472:DDP917487 CTS917472:CTT917487 CJW917472:CJX917487 CAA917472:CAB917487 BQE917472:BQF917487 BGI917472:BGJ917487 AWM917472:AWN917487 AMQ917472:AMR917487 ACU917472:ACV917487 SY917472:SZ917487 JC917472:JD917487 F917473:F917488 WVO851936:WVP851951 WLS851936:WLT851951 WBW851936:WBX851951 VSA851936:VSB851951 VIE851936:VIF851951 UYI851936:UYJ851951 UOM851936:UON851951 UEQ851936:UER851951 TUU851936:TUV851951 TKY851936:TKZ851951 TBC851936:TBD851951 SRG851936:SRH851951 SHK851936:SHL851951 RXO851936:RXP851951 RNS851936:RNT851951 RDW851936:RDX851951 QUA851936:QUB851951 QKE851936:QKF851951 QAI851936:QAJ851951 PQM851936:PQN851951 PGQ851936:PGR851951 OWU851936:OWV851951 OMY851936:OMZ851951 ODC851936:ODD851951 NTG851936:NTH851951 NJK851936:NJL851951 MZO851936:MZP851951 MPS851936:MPT851951 MFW851936:MFX851951 LWA851936:LWB851951 LME851936:LMF851951 LCI851936:LCJ851951 KSM851936:KSN851951 KIQ851936:KIR851951 JYU851936:JYV851951 JOY851936:JOZ851951 JFC851936:JFD851951 IVG851936:IVH851951 ILK851936:ILL851951 IBO851936:IBP851951 HRS851936:HRT851951 HHW851936:HHX851951 GYA851936:GYB851951 GOE851936:GOF851951 GEI851936:GEJ851951 FUM851936:FUN851951 FKQ851936:FKR851951 FAU851936:FAV851951 EQY851936:EQZ851951 EHC851936:EHD851951 DXG851936:DXH851951 DNK851936:DNL851951 DDO851936:DDP851951 CTS851936:CTT851951 CJW851936:CJX851951 CAA851936:CAB851951 BQE851936:BQF851951 BGI851936:BGJ851951 AWM851936:AWN851951 AMQ851936:AMR851951 ACU851936:ACV851951 SY851936:SZ851951 JC851936:JD851951 F851937:F851952 WVO786400:WVP786415 WLS786400:WLT786415 WBW786400:WBX786415 VSA786400:VSB786415 VIE786400:VIF786415 UYI786400:UYJ786415 UOM786400:UON786415 UEQ786400:UER786415 TUU786400:TUV786415 TKY786400:TKZ786415 TBC786400:TBD786415 SRG786400:SRH786415 SHK786400:SHL786415 RXO786400:RXP786415 RNS786400:RNT786415 RDW786400:RDX786415 QUA786400:QUB786415 QKE786400:QKF786415 QAI786400:QAJ786415 PQM786400:PQN786415 PGQ786400:PGR786415 OWU786400:OWV786415 OMY786400:OMZ786415 ODC786400:ODD786415 NTG786400:NTH786415 NJK786400:NJL786415 MZO786400:MZP786415 MPS786400:MPT786415 MFW786400:MFX786415 LWA786400:LWB786415 LME786400:LMF786415 LCI786400:LCJ786415 KSM786400:KSN786415 KIQ786400:KIR786415 JYU786400:JYV786415 JOY786400:JOZ786415 JFC786400:JFD786415 IVG786400:IVH786415 ILK786400:ILL786415 IBO786400:IBP786415 HRS786400:HRT786415 HHW786400:HHX786415 GYA786400:GYB786415 GOE786400:GOF786415 GEI786400:GEJ786415 FUM786400:FUN786415 FKQ786400:FKR786415 FAU786400:FAV786415 EQY786400:EQZ786415 EHC786400:EHD786415 DXG786400:DXH786415 DNK786400:DNL786415 DDO786400:DDP786415 CTS786400:CTT786415 CJW786400:CJX786415 CAA786400:CAB786415 BQE786400:BQF786415 BGI786400:BGJ786415 AWM786400:AWN786415 AMQ786400:AMR786415 ACU786400:ACV786415 SY786400:SZ786415 JC786400:JD786415 F786401:F786416 WVO720864:WVP720879 WLS720864:WLT720879 WBW720864:WBX720879 VSA720864:VSB720879 VIE720864:VIF720879 UYI720864:UYJ720879 UOM720864:UON720879 UEQ720864:UER720879 TUU720864:TUV720879 TKY720864:TKZ720879 TBC720864:TBD720879 SRG720864:SRH720879 SHK720864:SHL720879 RXO720864:RXP720879 RNS720864:RNT720879 RDW720864:RDX720879 QUA720864:QUB720879 QKE720864:QKF720879 QAI720864:QAJ720879 PQM720864:PQN720879 PGQ720864:PGR720879 OWU720864:OWV720879 OMY720864:OMZ720879 ODC720864:ODD720879 NTG720864:NTH720879 NJK720864:NJL720879 MZO720864:MZP720879 MPS720864:MPT720879 MFW720864:MFX720879 LWA720864:LWB720879 LME720864:LMF720879 LCI720864:LCJ720879 KSM720864:KSN720879 KIQ720864:KIR720879 JYU720864:JYV720879 JOY720864:JOZ720879 JFC720864:JFD720879 IVG720864:IVH720879 ILK720864:ILL720879 IBO720864:IBP720879 HRS720864:HRT720879 HHW720864:HHX720879 GYA720864:GYB720879 GOE720864:GOF720879 GEI720864:GEJ720879 FUM720864:FUN720879 FKQ720864:FKR720879 FAU720864:FAV720879 EQY720864:EQZ720879 EHC720864:EHD720879 DXG720864:DXH720879 DNK720864:DNL720879 DDO720864:DDP720879 CTS720864:CTT720879 CJW720864:CJX720879 CAA720864:CAB720879 BQE720864:BQF720879 BGI720864:BGJ720879 AWM720864:AWN720879 AMQ720864:AMR720879 ACU720864:ACV720879 SY720864:SZ720879 JC720864:JD720879 F720865:F720880 WVO655328:WVP655343 WLS655328:WLT655343 WBW655328:WBX655343 VSA655328:VSB655343 VIE655328:VIF655343 UYI655328:UYJ655343 UOM655328:UON655343 UEQ655328:UER655343 TUU655328:TUV655343 TKY655328:TKZ655343 TBC655328:TBD655343 SRG655328:SRH655343 SHK655328:SHL655343 RXO655328:RXP655343 RNS655328:RNT655343 RDW655328:RDX655343 QUA655328:QUB655343 QKE655328:QKF655343 QAI655328:QAJ655343 PQM655328:PQN655343 PGQ655328:PGR655343 OWU655328:OWV655343 OMY655328:OMZ655343 ODC655328:ODD655343 NTG655328:NTH655343 NJK655328:NJL655343 MZO655328:MZP655343 MPS655328:MPT655343 MFW655328:MFX655343 LWA655328:LWB655343 LME655328:LMF655343 LCI655328:LCJ655343 KSM655328:KSN655343 KIQ655328:KIR655343 JYU655328:JYV655343 JOY655328:JOZ655343 JFC655328:JFD655343 IVG655328:IVH655343 ILK655328:ILL655343 IBO655328:IBP655343 HRS655328:HRT655343 HHW655328:HHX655343 GYA655328:GYB655343 GOE655328:GOF655343 GEI655328:GEJ655343 FUM655328:FUN655343 FKQ655328:FKR655343 FAU655328:FAV655343 EQY655328:EQZ655343 EHC655328:EHD655343 DXG655328:DXH655343 DNK655328:DNL655343 DDO655328:DDP655343 CTS655328:CTT655343 CJW655328:CJX655343 CAA655328:CAB655343 BQE655328:BQF655343 BGI655328:BGJ655343 AWM655328:AWN655343 AMQ655328:AMR655343 ACU655328:ACV655343 SY655328:SZ655343 JC655328:JD655343 F655329:F655344 WVO589792:WVP589807 WLS589792:WLT589807 WBW589792:WBX589807 VSA589792:VSB589807 VIE589792:VIF589807 UYI589792:UYJ589807 UOM589792:UON589807 UEQ589792:UER589807 TUU589792:TUV589807 TKY589792:TKZ589807 TBC589792:TBD589807 SRG589792:SRH589807 SHK589792:SHL589807 RXO589792:RXP589807 RNS589792:RNT589807 RDW589792:RDX589807 QUA589792:QUB589807 QKE589792:QKF589807 QAI589792:QAJ589807 PQM589792:PQN589807 PGQ589792:PGR589807 OWU589792:OWV589807 OMY589792:OMZ589807 ODC589792:ODD589807 NTG589792:NTH589807 NJK589792:NJL589807 MZO589792:MZP589807 MPS589792:MPT589807 MFW589792:MFX589807 LWA589792:LWB589807 LME589792:LMF589807 LCI589792:LCJ589807 KSM589792:KSN589807 KIQ589792:KIR589807 JYU589792:JYV589807 JOY589792:JOZ589807 JFC589792:JFD589807 IVG589792:IVH589807 ILK589792:ILL589807 IBO589792:IBP589807 HRS589792:HRT589807 HHW589792:HHX589807 GYA589792:GYB589807 GOE589792:GOF589807 GEI589792:GEJ589807 FUM589792:FUN589807 FKQ589792:FKR589807 FAU589792:FAV589807 EQY589792:EQZ589807 EHC589792:EHD589807 DXG589792:DXH589807 DNK589792:DNL589807 DDO589792:DDP589807 CTS589792:CTT589807 CJW589792:CJX589807 CAA589792:CAB589807 BQE589792:BQF589807 BGI589792:BGJ589807 AWM589792:AWN589807 AMQ589792:AMR589807 ACU589792:ACV589807 SY589792:SZ589807 JC589792:JD589807 F589793:F589808 WVO524256:WVP524271 WLS524256:WLT524271 WBW524256:WBX524271 VSA524256:VSB524271 VIE524256:VIF524271 UYI524256:UYJ524271 UOM524256:UON524271 UEQ524256:UER524271 TUU524256:TUV524271 TKY524256:TKZ524271 TBC524256:TBD524271 SRG524256:SRH524271 SHK524256:SHL524271 RXO524256:RXP524271 RNS524256:RNT524271 RDW524256:RDX524271 QUA524256:QUB524271 QKE524256:QKF524271 QAI524256:QAJ524271 PQM524256:PQN524271 PGQ524256:PGR524271 OWU524256:OWV524271 OMY524256:OMZ524271 ODC524256:ODD524271 NTG524256:NTH524271 NJK524256:NJL524271 MZO524256:MZP524271 MPS524256:MPT524271 MFW524256:MFX524271 LWA524256:LWB524271 LME524256:LMF524271 LCI524256:LCJ524271 KSM524256:KSN524271 KIQ524256:KIR524271 JYU524256:JYV524271 JOY524256:JOZ524271 JFC524256:JFD524271 IVG524256:IVH524271 ILK524256:ILL524271 IBO524256:IBP524271 HRS524256:HRT524271 HHW524256:HHX524271 GYA524256:GYB524271 GOE524256:GOF524271 GEI524256:GEJ524271 FUM524256:FUN524271 FKQ524256:FKR524271 FAU524256:FAV524271 EQY524256:EQZ524271 EHC524256:EHD524271 DXG524256:DXH524271 DNK524256:DNL524271 DDO524256:DDP524271 CTS524256:CTT524271 CJW524256:CJX524271 CAA524256:CAB524271 BQE524256:BQF524271 BGI524256:BGJ524271 AWM524256:AWN524271 AMQ524256:AMR524271 ACU524256:ACV524271 SY524256:SZ524271 JC524256:JD524271 F524257:F524272 WVO458720:WVP458735 WLS458720:WLT458735 WBW458720:WBX458735 VSA458720:VSB458735 VIE458720:VIF458735 UYI458720:UYJ458735 UOM458720:UON458735 UEQ458720:UER458735 TUU458720:TUV458735 TKY458720:TKZ458735 TBC458720:TBD458735 SRG458720:SRH458735 SHK458720:SHL458735 RXO458720:RXP458735 RNS458720:RNT458735 RDW458720:RDX458735 QUA458720:QUB458735 QKE458720:QKF458735 QAI458720:QAJ458735 PQM458720:PQN458735 PGQ458720:PGR458735 OWU458720:OWV458735 OMY458720:OMZ458735 ODC458720:ODD458735 NTG458720:NTH458735 NJK458720:NJL458735 MZO458720:MZP458735 MPS458720:MPT458735 MFW458720:MFX458735 LWA458720:LWB458735 LME458720:LMF458735 LCI458720:LCJ458735 KSM458720:KSN458735 KIQ458720:KIR458735 JYU458720:JYV458735 JOY458720:JOZ458735 JFC458720:JFD458735 IVG458720:IVH458735 ILK458720:ILL458735 IBO458720:IBP458735 HRS458720:HRT458735 HHW458720:HHX458735 GYA458720:GYB458735 GOE458720:GOF458735 GEI458720:GEJ458735 FUM458720:FUN458735 FKQ458720:FKR458735 FAU458720:FAV458735 EQY458720:EQZ458735 EHC458720:EHD458735 DXG458720:DXH458735 DNK458720:DNL458735 DDO458720:DDP458735 CTS458720:CTT458735 CJW458720:CJX458735 CAA458720:CAB458735 BQE458720:BQF458735 BGI458720:BGJ458735 AWM458720:AWN458735 AMQ458720:AMR458735 ACU458720:ACV458735 SY458720:SZ458735 JC458720:JD458735 F458721:F458736 WVO393184:WVP393199 WLS393184:WLT393199 WBW393184:WBX393199 VSA393184:VSB393199 VIE393184:VIF393199 UYI393184:UYJ393199 UOM393184:UON393199 UEQ393184:UER393199 TUU393184:TUV393199 TKY393184:TKZ393199 TBC393184:TBD393199 SRG393184:SRH393199 SHK393184:SHL393199 RXO393184:RXP393199 RNS393184:RNT393199 RDW393184:RDX393199 QUA393184:QUB393199 QKE393184:QKF393199 QAI393184:QAJ393199 PQM393184:PQN393199 PGQ393184:PGR393199 OWU393184:OWV393199 OMY393184:OMZ393199 ODC393184:ODD393199 NTG393184:NTH393199 NJK393184:NJL393199 MZO393184:MZP393199 MPS393184:MPT393199 MFW393184:MFX393199 LWA393184:LWB393199 LME393184:LMF393199 LCI393184:LCJ393199 KSM393184:KSN393199 KIQ393184:KIR393199 JYU393184:JYV393199 JOY393184:JOZ393199 JFC393184:JFD393199 IVG393184:IVH393199 ILK393184:ILL393199 IBO393184:IBP393199 HRS393184:HRT393199 HHW393184:HHX393199 GYA393184:GYB393199 GOE393184:GOF393199 GEI393184:GEJ393199 FUM393184:FUN393199 FKQ393184:FKR393199 FAU393184:FAV393199 EQY393184:EQZ393199 EHC393184:EHD393199 DXG393184:DXH393199 DNK393184:DNL393199 DDO393184:DDP393199 CTS393184:CTT393199 CJW393184:CJX393199 CAA393184:CAB393199 BQE393184:BQF393199 BGI393184:BGJ393199 AWM393184:AWN393199 AMQ393184:AMR393199 ACU393184:ACV393199 SY393184:SZ393199 JC393184:JD393199 F393185:F393200 WVO327648:WVP327663 WLS327648:WLT327663 WBW327648:WBX327663 VSA327648:VSB327663 VIE327648:VIF327663 UYI327648:UYJ327663 UOM327648:UON327663 UEQ327648:UER327663 TUU327648:TUV327663 TKY327648:TKZ327663 TBC327648:TBD327663 SRG327648:SRH327663 SHK327648:SHL327663 RXO327648:RXP327663 RNS327648:RNT327663 RDW327648:RDX327663 QUA327648:QUB327663 QKE327648:QKF327663 QAI327648:QAJ327663 PQM327648:PQN327663 PGQ327648:PGR327663 OWU327648:OWV327663 OMY327648:OMZ327663 ODC327648:ODD327663 NTG327648:NTH327663 NJK327648:NJL327663 MZO327648:MZP327663 MPS327648:MPT327663 MFW327648:MFX327663 LWA327648:LWB327663 LME327648:LMF327663 LCI327648:LCJ327663 KSM327648:KSN327663 KIQ327648:KIR327663 JYU327648:JYV327663 JOY327648:JOZ327663 JFC327648:JFD327663 IVG327648:IVH327663 ILK327648:ILL327663 IBO327648:IBP327663 HRS327648:HRT327663 HHW327648:HHX327663 GYA327648:GYB327663 GOE327648:GOF327663 GEI327648:GEJ327663 FUM327648:FUN327663 FKQ327648:FKR327663 FAU327648:FAV327663 EQY327648:EQZ327663 EHC327648:EHD327663 DXG327648:DXH327663 DNK327648:DNL327663 DDO327648:DDP327663 CTS327648:CTT327663 CJW327648:CJX327663 CAA327648:CAB327663 BQE327648:BQF327663 BGI327648:BGJ327663 AWM327648:AWN327663 AMQ327648:AMR327663 ACU327648:ACV327663 SY327648:SZ327663 JC327648:JD327663 F327649:F327664 WVO262112:WVP262127 WLS262112:WLT262127 WBW262112:WBX262127 VSA262112:VSB262127 VIE262112:VIF262127 UYI262112:UYJ262127 UOM262112:UON262127 UEQ262112:UER262127 TUU262112:TUV262127 TKY262112:TKZ262127 TBC262112:TBD262127 SRG262112:SRH262127 SHK262112:SHL262127 RXO262112:RXP262127 RNS262112:RNT262127 RDW262112:RDX262127 QUA262112:QUB262127 QKE262112:QKF262127 QAI262112:QAJ262127 PQM262112:PQN262127 PGQ262112:PGR262127 OWU262112:OWV262127 OMY262112:OMZ262127 ODC262112:ODD262127 NTG262112:NTH262127 NJK262112:NJL262127 MZO262112:MZP262127 MPS262112:MPT262127 MFW262112:MFX262127 LWA262112:LWB262127 LME262112:LMF262127 LCI262112:LCJ262127 KSM262112:KSN262127 KIQ262112:KIR262127 JYU262112:JYV262127 JOY262112:JOZ262127 JFC262112:JFD262127 IVG262112:IVH262127 ILK262112:ILL262127 IBO262112:IBP262127 HRS262112:HRT262127 HHW262112:HHX262127 GYA262112:GYB262127 GOE262112:GOF262127 GEI262112:GEJ262127 FUM262112:FUN262127 FKQ262112:FKR262127 FAU262112:FAV262127 EQY262112:EQZ262127 EHC262112:EHD262127 DXG262112:DXH262127 DNK262112:DNL262127 DDO262112:DDP262127 CTS262112:CTT262127 CJW262112:CJX262127 CAA262112:CAB262127 BQE262112:BQF262127 BGI262112:BGJ262127 AWM262112:AWN262127 AMQ262112:AMR262127 ACU262112:ACV262127 SY262112:SZ262127 JC262112:JD262127 F262113:F262128 WVO196576:WVP196591 WLS196576:WLT196591 WBW196576:WBX196591 VSA196576:VSB196591 VIE196576:VIF196591 UYI196576:UYJ196591 UOM196576:UON196591 UEQ196576:UER196591 TUU196576:TUV196591 TKY196576:TKZ196591 TBC196576:TBD196591 SRG196576:SRH196591 SHK196576:SHL196591 RXO196576:RXP196591 RNS196576:RNT196591 RDW196576:RDX196591 QUA196576:QUB196591 QKE196576:QKF196591 QAI196576:QAJ196591 PQM196576:PQN196591 PGQ196576:PGR196591 OWU196576:OWV196591 OMY196576:OMZ196591 ODC196576:ODD196591 NTG196576:NTH196591 NJK196576:NJL196591 MZO196576:MZP196591 MPS196576:MPT196591 MFW196576:MFX196591 LWA196576:LWB196591 LME196576:LMF196591 LCI196576:LCJ196591 KSM196576:KSN196591 KIQ196576:KIR196591 JYU196576:JYV196591 JOY196576:JOZ196591 JFC196576:JFD196591 IVG196576:IVH196591 ILK196576:ILL196591 IBO196576:IBP196591 HRS196576:HRT196591 HHW196576:HHX196591 GYA196576:GYB196591 GOE196576:GOF196591 GEI196576:GEJ196591 FUM196576:FUN196591 FKQ196576:FKR196591 FAU196576:FAV196591 EQY196576:EQZ196591 EHC196576:EHD196591 DXG196576:DXH196591 DNK196576:DNL196591 DDO196576:DDP196591 CTS196576:CTT196591 CJW196576:CJX196591 CAA196576:CAB196591 BQE196576:BQF196591 BGI196576:BGJ196591 AWM196576:AWN196591 AMQ196576:AMR196591 ACU196576:ACV196591 SY196576:SZ196591 JC196576:JD196591 F196577:F196592 WVO131040:WVP131055 WLS131040:WLT131055 WBW131040:WBX131055 VSA131040:VSB131055 VIE131040:VIF131055 UYI131040:UYJ131055 UOM131040:UON131055 UEQ131040:UER131055 TUU131040:TUV131055 TKY131040:TKZ131055 TBC131040:TBD131055 SRG131040:SRH131055 SHK131040:SHL131055 RXO131040:RXP131055 RNS131040:RNT131055 RDW131040:RDX131055 QUA131040:QUB131055 QKE131040:QKF131055 QAI131040:QAJ131055 PQM131040:PQN131055 PGQ131040:PGR131055 OWU131040:OWV131055 OMY131040:OMZ131055 ODC131040:ODD131055 NTG131040:NTH131055 NJK131040:NJL131055 MZO131040:MZP131055 MPS131040:MPT131055 MFW131040:MFX131055 LWA131040:LWB131055 LME131040:LMF131055 LCI131040:LCJ131055 KSM131040:KSN131055 KIQ131040:KIR131055 JYU131040:JYV131055 JOY131040:JOZ131055 JFC131040:JFD131055 IVG131040:IVH131055 ILK131040:ILL131055 IBO131040:IBP131055 HRS131040:HRT131055 HHW131040:HHX131055 GYA131040:GYB131055 GOE131040:GOF131055 GEI131040:GEJ131055 FUM131040:FUN131055 FKQ131040:FKR131055 FAU131040:FAV131055 EQY131040:EQZ131055 EHC131040:EHD131055 DXG131040:DXH131055 DNK131040:DNL131055 DDO131040:DDP131055 CTS131040:CTT131055 CJW131040:CJX131055 CAA131040:CAB131055 BQE131040:BQF131055 BGI131040:BGJ131055 AWM131040:AWN131055 AMQ131040:AMR131055 ACU131040:ACV131055 SY131040:SZ131055 JC131040:JD131055 F131041:F131056 WVO65504:WVP65519 WLS65504:WLT65519 WBW65504:WBX65519 VSA65504:VSB65519 VIE65504:VIF65519 UYI65504:UYJ65519 UOM65504:UON65519 UEQ65504:UER65519 TUU65504:TUV65519 TKY65504:TKZ65519 TBC65504:TBD65519 SRG65504:SRH65519 SHK65504:SHL65519 RXO65504:RXP65519 RNS65504:RNT65519 RDW65504:RDX65519 QUA65504:QUB65519 QKE65504:QKF65519 QAI65504:QAJ65519 PQM65504:PQN65519 PGQ65504:PGR65519 OWU65504:OWV65519 OMY65504:OMZ65519 ODC65504:ODD65519 NTG65504:NTH65519 NJK65504:NJL65519 MZO65504:MZP65519 MPS65504:MPT65519 MFW65504:MFX65519 LWA65504:LWB65519 LME65504:LMF65519 LCI65504:LCJ65519 KSM65504:KSN65519 KIQ65504:KIR65519 JYU65504:JYV65519 JOY65504:JOZ65519 JFC65504:JFD65519 IVG65504:IVH65519 ILK65504:ILL65519 IBO65504:IBP65519 HRS65504:HRT65519 HHW65504:HHX65519 GYA65504:GYB65519 GOE65504:GOF65519 GEI65504:GEJ65519 FUM65504:FUN65519 FKQ65504:FKR65519 FAU65504:FAV65519 EQY65504:EQZ65519 EHC65504:EHD65519 DXG65504:DXH65519 DNK65504:DNL65519 DDO65504:DDP65519 CTS65504:CTT65519 CJW65504:CJX65519 CAA65504:CAB65519 BQE65504:BQF65519 BGI65504:BGJ65519 AWM65504:AWN65519 AMQ65504:AMR65519 ACU65504:ACV65519 SY65504:SZ65519 JC65504:JD65519 WLI14:WLJ17 WBM14:WBN17 VRQ14:VRR17 VHU14:VHV17 UXY14:UXZ17 UOC14:UOD17 UEG14:UEH17 TUK14:TUL17 TKO14:TKP17 TAS14:TAT17 SQW14:SQX17 SHA14:SHB17 RXE14:RXF17 RNI14:RNJ17 RDM14:RDN17 QTQ14:QTR17 QJU14:QJV17 PZY14:PZZ17 PQC14:PQD17 PGG14:PGH17 OWK14:OWL17 OMO14:OMP17 OCS14:OCT17 NSW14:NSX17 NJA14:NJB17 MZE14:MZF17 MPI14:MPJ17 MFM14:MFN17 LVQ14:LVR17 LLU14:LLV17 LBY14:LBZ17 KSC14:KSD17 KIG14:KIH17 JYK14:JYL17 JOO14:JOP17 JES14:JET17 IUW14:IUX17 ILA14:ILB17 IBE14:IBF17 HRI14:HRJ17 HHM14:HHN17 GXQ14:GXR17 GNU14:GNV17 GDY14:GDZ17 FUC14:FUD17 FKG14:FKH17 FAK14:FAL17 EQO14:EQP17 EGS14:EGT17 DWW14:DWX17 DNA14:DNB17 DDE14:DDF17 CTI14:CTJ17 CJM14:CJN17 BZQ14:BZR17 BPU14:BPV17 BFY14:BFZ17 AWC14:AWD17 AMG14:AMH17 ACK14:ACL17 SO14:SP17 IS14:IT17 WVE14:WVF17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C65496:C65519 IZ65495:IZ65518 SV65495:SV65518 ACR65495:ACR65518 AMN65495:AMN65518 AWJ65495:AWJ65518 BGF65495:BGF65518 BQB65495:BQB65518 BZX65495:BZX65518 CJT65495:CJT65518 CTP65495:CTP65518 DDL65495:DDL65518 DNH65495:DNH65518 DXD65495:DXD65518 EGZ65495:EGZ65518 EQV65495:EQV65518 FAR65495:FAR65518 FKN65495:FKN65518 FUJ65495:FUJ65518 GEF65495:GEF65518 GOB65495:GOB65518 GXX65495:GXX65518 HHT65495:HHT65518 HRP65495:HRP65518 IBL65495:IBL65518 ILH65495:ILH65518 IVD65495:IVD65518 JEZ65495:JEZ65518 JOV65495:JOV65518 JYR65495:JYR65518 KIN65495:KIN65518 KSJ65495:KSJ65518 LCF65495:LCF65518 LMB65495:LMB65518 LVX65495:LVX65518 MFT65495:MFT65518 MPP65495:MPP65518 MZL65495:MZL65518 NJH65495:NJH65518 NTD65495:NTD65518 OCZ65495:OCZ65518 OMV65495:OMV65518 OWR65495:OWR65518 PGN65495:PGN65518 PQJ65495:PQJ65518 QAF65495:QAF65518 QKB65495:QKB65518 QTX65495:QTX65518 RDT65495:RDT65518 RNP65495:RNP65518 RXL65495:RXL65518 SHH65495:SHH65518 SRD65495:SRD65518 TAZ65495:TAZ65518 TKV65495:TKV65518 TUR65495:TUR65518 UEN65495:UEN65518 UOJ65495:UOJ65518 UYF65495:UYF65518 VIB65495:VIB65518 VRX65495:VRX65518 WBT65495:WBT65518 WLP65495:WLP65518 WVL65495:WVL65518 C131032:C131055 IZ131031:IZ131054 SV131031:SV131054 ACR131031:ACR131054 AMN131031:AMN131054 AWJ131031:AWJ131054 BGF131031:BGF131054 BQB131031:BQB131054 BZX131031:BZX131054 CJT131031:CJT131054 CTP131031:CTP131054 DDL131031:DDL131054 DNH131031:DNH131054 DXD131031:DXD131054 EGZ131031:EGZ131054 EQV131031:EQV131054 FAR131031:FAR131054 FKN131031:FKN131054 FUJ131031:FUJ131054 GEF131031:GEF131054 GOB131031:GOB131054 GXX131031:GXX131054 HHT131031:HHT131054 HRP131031:HRP131054 IBL131031:IBL131054 ILH131031:ILH131054 IVD131031:IVD131054 JEZ131031:JEZ131054 JOV131031:JOV131054 JYR131031:JYR131054 KIN131031:KIN131054 KSJ131031:KSJ131054 LCF131031:LCF131054 LMB131031:LMB131054 LVX131031:LVX131054 MFT131031:MFT131054 MPP131031:MPP131054 MZL131031:MZL131054 NJH131031:NJH131054 NTD131031:NTD131054 OCZ131031:OCZ131054 OMV131031:OMV131054 OWR131031:OWR131054 PGN131031:PGN131054 PQJ131031:PQJ131054 QAF131031:QAF131054 QKB131031:QKB131054 QTX131031:QTX131054 RDT131031:RDT131054 RNP131031:RNP131054 RXL131031:RXL131054 SHH131031:SHH131054 SRD131031:SRD131054 TAZ131031:TAZ131054 TKV131031:TKV131054 TUR131031:TUR131054 UEN131031:UEN131054 UOJ131031:UOJ131054 UYF131031:UYF131054 VIB131031:VIB131054 VRX131031:VRX131054 WBT131031:WBT131054 WLP131031:WLP131054 WVL131031:WVL131054 C196568:C196591 IZ196567:IZ196590 SV196567:SV196590 ACR196567:ACR196590 AMN196567:AMN196590 AWJ196567:AWJ196590 BGF196567:BGF196590 BQB196567:BQB196590 BZX196567:BZX196590 CJT196567:CJT196590 CTP196567:CTP196590 DDL196567:DDL196590 DNH196567:DNH196590 DXD196567:DXD196590 EGZ196567:EGZ196590 EQV196567:EQV196590 FAR196567:FAR196590 FKN196567:FKN196590 FUJ196567:FUJ196590 GEF196567:GEF196590 GOB196567:GOB196590 GXX196567:GXX196590 HHT196567:HHT196590 HRP196567:HRP196590 IBL196567:IBL196590 ILH196567:ILH196590 IVD196567:IVD196590 JEZ196567:JEZ196590 JOV196567:JOV196590 JYR196567:JYR196590 KIN196567:KIN196590 KSJ196567:KSJ196590 LCF196567:LCF196590 LMB196567:LMB196590 LVX196567:LVX196590 MFT196567:MFT196590 MPP196567:MPP196590 MZL196567:MZL196590 NJH196567:NJH196590 NTD196567:NTD196590 OCZ196567:OCZ196590 OMV196567:OMV196590 OWR196567:OWR196590 PGN196567:PGN196590 PQJ196567:PQJ196590 QAF196567:QAF196590 QKB196567:QKB196590 QTX196567:QTX196590 RDT196567:RDT196590 RNP196567:RNP196590 RXL196567:RXL196590 SHH196567:SHH196590 SRD196567:SRD196590 TAZ196567:TAZ196590 TKV196567:TKV196590 TUR196567:TUR196590 UEN196567:UEN196590 UOJ196567:UOJ196590 UYF196567:UYF196590 VIB196567:VIB196590 VRX196567:VRX196590 WBT196567:WBT196590 WLP196567:WLP196590 WVL196567:WVL196590 C262104:C262127 IZ262103:IZ262126 SV262103:SV262126 ACR262103:ACR262126 AMN262103:AMN262126 AWJ262103:AWJ262126 BGF262103:BGF262126 BQB262103:BQB262126 BZX262103:BZX262126 CJT262103:CJT262126 CTP262103:CTP262126 DDL262103:DDL262126 DNH262103:DNH262126 DXD262103:DXD262126 EGZ262103:EGZ262126 EQV262103:EQV262126 FAR262103:FAR262126 FKN262103:FKN262126 FUJ262103:FUJ262126 GEF262103:GEF262126 GOB262103:GOB262126 GXX262103:GXX262126 HHT262103:HHT262126 HRP262103:HRP262126 IBL262103:IBL262126 ILH262103:ILH262126 IVD262103:IVD262126 JEZ262103:JEZ262126 JOV262103:JOV262126 JYR262103:JYR262126 KIN262103:KIN262126 KSJ262103:KSJ262126 LCF262103:LCF262126 LMB262103:LMB262126 LVX262103:LVX262126 MFT262103:MFT262126 MPP262103:MPP262126 MZL262103:MZL262126 NJH262103:NJH262126 NTD262103:NTD262126 OCZ262103:OCZ262126 OMV262103:OMV262126 OWR262103:OWR262126 PGN262103:PGN262126 PQJ262103:PQJ262126 QAF262103:QAF262126 QKB262103:QKB262126 QTX262103:QTX262126 RDT262103:RDT262126 RNP262103:RNP262126 RXL262103:RXL262126 SHH262103:SHH262126 SRD262103:SRD262126 TAZ262103:TAZ262126 TKV262103:TKV262126 TUR262103:TUR262126 UEN262103:UEN262126 UOJ262103:UOJ262126 UYF262103:UYF262126 VIB262103:VIB262126 VRX262103:VRX262126 WBT262103:WBT262126 WLP262103:WLP262126 WVL262103:WVL262126 C327640:C327663 IZ327639:IZ327662 SV327639:SV327662 ACR327639:ACR327662 AMN327639:AMN327662 AWJ327639:AWJ327662 BGF327639:BGF327662 BQB327639:BQB327662 BZX327639:BZX327662 CJT327639:CJT327662 CTP327639:CTP327662 DDL327639:DDL327662 DNH327639:DNH327662 DXD327639:DXD327662 EGZ327639:EGZ327662 EQV327639:EQV327662 FAR327639:FAR327662 FKN327639:FKN327662 FUJ327639:FUJ327662 GEF327639:GEF327662 GOB327639:GOB327662 GXX327639:GXX327662 HHT327639:HHT327662 HRP327639:HRP327662 IBL327639:IBL327662 ILH327639:ILH327662 IVD327639:IVD327662 JEZ327639:JEZ327662 JOV327639:JOV327662 JYR327639:JYR327662 KIN327639:KIN327662 KSJ327639:KSJ327662 LCF327639:LCF327662 LMB327639:LMB327662 LVX327639:LVX327662 MFT327639:MFT327662 MPP327639:MPP327662 MZL327639:MZL327662 NJH327639:NJH327662 NTD327639:NTD327662 OCZ327639:OCZ327662 OMV327639:OMV327662 OWR327639:OWR327662 PGN327639:PGN327662 PQJ327639:PQJ327662 QAF327639:QAF327662 QKB327639:QKB327662 QTX327639:QTX327662 RDT327639:RDT327662 RNP327639:RNP327662 RXL327639:RXL327662 SHH327639:SHH327662 SRD327639:SRD327662 TAZ327639:TAZ327662 TKV327639:TKV327662 TUR327639:TUR327662 UEN327639:UEN327662 UOJ327639:UOJ327662 UYF327639:UYF327662 VIB327639:VIB327662 VRX327639:VRX327662 WBT327639:WBT327662 WLP327639:WLP327662 WVL327639:WVL327662 C393176:C393199 IZ393175:IZ393198 SV393175:SV393198 ACR393175:ACR393198 AMN393175:AMN393198 AWJ393175:AWJ393198 BGF393175:BGF393198 BQB393175:BQB393198 BZX393175:BZX393198 CJT393175:CJT393198 CTP393175:CTP393198 DDL393175:DDL393198 DNH393175:DNH393198 DXD393175:DXD393198 EGZ393175:EGZ393198 EQV393175:EQV393198 FAR393175:FAR393198 FKN393175:FKN393198 FUJ393175:FUJ393198 GEF393175:GEF393198 GOB393175:GOB393198 GXX393175:GXX393198 HHT393175:HHT393198 HRP393175:HRP393198 IBL393175:IBL393198 ILH393175:ILH393198 IVD393175:IVD393198 JEZ393175:JEZ393198 JOV393175:JOV393198 JYR393175:JYR393198 KIN393175:KIN393198 KSJ393175:KSJ393198 LCF393175:LCF393198 LMB393175:LMB393198 LVX393175:LVX393198 MFT393175:MFT393198 MPP393175:MPP393198 MZL393175:MZL393198 NJH393175:NJH393198 NTD393175:NTD393198 OCZ393175:OCZ393198 OMV393175:OMV393198 OWR393175:OWR393198 PGN393175:PGN393198 PQJ393175:PQJ393198 QAF393175:QAF393198 QKB393175:QKB393198 QTX393175:QTX393198 RDT393175:RDT393198 RNP393175:RNP393198 RXL393175:RXL393198 SHH393175:SHH393198 SRD393175:SRD393198 TAZ393175:TAZ393198 TKV393175:TKV393198 TUR393175:TUR393198 UEN393175:UEN393198 UOJ393175:UOJ393198 UYF393175:UYF393198 VIB393175:VIB393198 VRX393175:VRX393198 WBT393175:WBT393198 WLP393175:WLP393198 WVL393175:WVL393198 C458712:C458735 IZ458711:IZ458734 SV458711:SV458734 ACR458711:ACR458734 AMN458711:AMN458734 AWJ458711:AWJ458734 BGF458711:BGF458734 BQB458711:BQB458734 BZX458711:BZX458734 CJT458711:CJT458734 CTP458711:CTP458734 DDL458711:DDL458734 DNH458711:DNH458734 DXD458711:DXD458734 EGZ458711:EGZ458734 EQV458711:EQV458734 FAR458711:FAR458734 FKN458711:FKN458734 FUJ458711:FUJ458734 GEF458711:GEF458734 GOB458711:GOB458734 GXX458711:GXX458734 HHT458711:HHT458734 HRP458711:HRP458734 IBL458711:IBL458734 ILH458711:ILH458734 IVD458711:IVD458734 JEZ458711:JEZ458734 JOV458711:JOV458734 JYR458711:JYR458734 KIN458711:KIN458734 KSJ458711:KSJ458734 LCF458711:LCF458734 LMB458711:LMB458734 LVX458711:LVX458734 MFT458711:MFT458734 MPP458711:MPP458734 MZL458711:MZL458734 NJH458711:NJH458734 NTD458711:NTD458734 OCZ458711:OCZ458734 OMV458711:OMV458734 OWR458711:OWR458734 PGN458711:PGN458734 PQJ458711:PQJ458734 QAF458711:QAF458734 QKB458711:QKB458734 QTX458711:QTX458734 RDT458711:RDT458734 RNP458711:RNP458734 RXL458711:RXL458734 SHH458711:SHH458734 SRD458711:SRD458734 TAZ458711:TAZ458734 TKV458711:TKV458734 TUR458711:TUR458734 UEN458711:UEN458734 UOJ458711:UOJ458734 UYF458711:UYF458734 VIB458711:VIB458734 VRX458711:VRX458734 WBT458711:WBT458734 WLP458711:WLP458734 WVL458711:WVL458734 C524248:C524271 IZ524247:IZ524270 SV524247:SV524270 ACR524247:ACR524270 AMN524247:AMN524270 AWJ524247:AWJ524270 BGF524247:BGF524270 BQB524247:BQB524270 BZX524247:BZX524270 CJT524247:CJT524270 CTP524247:CTP524270 DDL524247:DDL524270 DNH524247:DNH524270 DXD524247:DXD524270 EGZ524247:EGZ524270 EQV524247:EQV524270 FAR524247:FAR524270 FKN524247:FKN524270 FUJ524247:FUJ524270 GEF524247:GEF524270 GOB524247:GOB524270 GXX524247:GXX524270 HHT524247:HHT524270 HRP524247:HRP524270 IBL524247:IBL524270 ILH524247:ILH524270 IVD524247:IVD524270 JEZ524247:JEZ524270 JOV524247:JOV524270 JYR524247:JYR524270 KIN524247:KIN524270 KSJ524247:KSJ524270 LCF524247:LCF524270 LMB524247:LMB524270 LVX524247:LVX524270 MFT524247:MFT524270 MPP524247:MPP524270 MZL524247:MZL524270 NJH524247:NJH524270 NTD524247:NTD524270 OCZ524247:OCZ524270 OMV524247:OMV524270 OWR524247:OWR524270 PGN524247:PGN524270 PQJ524247:PQJ524270 QAF524247:QAF524270 QKB524247:QKB524270 QTX524247:QTX524270 RDT524247:RDT524270 RNP524247:RNP524270 RXL524247:RXL524270 SHH524247:SHH524270 SRD524247:SRD524270 TAZ524247:TAZ524270 TKV524247:TKV524270 TUR524247:TUR524270 UEN524247:UEN524270 UOJ524247:UOJ524270 UYF524247:UYF524270 VIB524247:VIB524270 VRX524247:VRX524270 WBT524247:WBT524270 WLP524247:WLP524270 WVL524247:WVL524270 C589784:C589807 IZ589783:IZ589806 SV589783:SV589806 ACR589783:ACR589806 AMN589783:AMN589806 AWJ589783:AWJ589806 BGF589783:BGF589806 BQB589783:BQB589806 BZX589783:BZX589806 CJT589783:CJT589806 CTP589783:CTP589806 DDL589783:DDL589806 DNH589783:DNH589806 DXD589783:DXD589806 EGZ589783:EGZ589806 EQV589783:EQV589806 FAR589783:FAR589806 FKN589783:FKN589806 FUJ589783:FUJ589806 GEF589783:GEF589806 GOB589783:GOB589806 GXX589783:GXX589806 HHT589783:HHT589806 HRP589783:HRP589806 IBL589783:IBL589806 ILH589783:ILH589806 IVD589783:IVD589806 JEZ589783:JEZ589806 JOV589783:JOV589806 JYR589783:JYR589806 KIN589783:KIN589806 KSJ589783:KSJ589806 LCF589783:LCF589806 LMB589783:LMB589806 LVX589783:LVX589806 MFT589783:MFT589806 MPP589783:MPP589806 MZL589783:MZL589806 NJH589783:NJH589806 NTD589783:NTD589806 OCZ589783:OCZ589806 OMV589783:OMV589806 OWR589783:OWR589806 PGN589783:PGN589806 PQJ589783:PQJ589806 QAF589783:QAF589806 QKB589783:QKB589806 QTX589783:QTX589806 RDT589783:RDT589806 RNP589783:RNP589806 RXL589783:RXL589806 SHH589783:SHH589806 SRD589783:SRD589806 TAZ589783:TAZ589806 TKV589783:TKV589806 TUR589783:TUR589806 UEN589783:UEN589806 UOJ589783:UOJ589806 UYF589783:UYF589806 VIB589783:VIB589806 VRX589783:VRX589806 WBT589783:WBT589806 WLP589783:WLP589806 WVL589783:WVL589806 C655320:C655343 IZ655319:IZ655342 SV655319:SV655342 ACR655319:ACR655342 AMN655319:AMN655342 AWJ655319:AWJ655342 BGF655319:BGF655342 BQB655319:BQB655342 BZX655319:BZX655342 CJT655319:CJT655342 CTP655319:CTP655342 DDL655319:DDL655342 DNH655319:DNH655342 DXD655319:DXD655342 EGZ655319:EGZ655342 EQV655319:EQV655342 FAR655319:FAR655342 FKN655319:FKN655342 FUJ655319:FUJ655342 GEF655319:GEF655342 GOB655319:GOB655342 GXX655319:GXX655342 HHT655319:HHT655342 HRP655319:HRP655342 IBL655319:IBL655342 ILH655319:ILH655342 IVD655319:IVD655342 JEZ655319:JEZ655342 JOV655319:JOV655342 JYR655319:JYR655342 KIN655319:KIN655342 KSJ655319:KSJ655342 LCF655319:LCF655342 LMB655319:LMB655342 LVX655319:LVX655342 MFT655319:MFT655342 MPP655319:MPP655342 MZL655319:MZL655342 NJH655319:NJH655342 NTD655319:NTD655342 OCZ655319:OCZ655342 OMV655319:OMV655342 OWR655319:OWR655342 PGN655319:PGN655342 PQJ655319:PQJ655342 QAF655319:QAF655342 QKB655319:QKB655342 QTX655319:QTX655342 RDT655319:RDT655342 RNP655319:RNP655342 RXL655319:RXL655342 SHH655319:SHH655342 SRD655319:SRD655342 TAZ655319:TAZ655342 TKV655319:TKV655342 TUR655319:TUR655342 UEN655319:UEN655342 UOJ655319:UOJ655342 UYF655319:UYF655342 VIB655319:VIB655342 VRX655319:VRX655342 WBT655319:WBT655342 WLP655319:WLP655342 WVL655319:WVL655342 C720856:C720879 IZ720855:IZ720878 SV720855:SV720878 ACR720855:ACR720878 AMN720855:AMN720878 AWJ720855:AWJ720878 BGF720855:BGF720878 BQB720855:BQB720878 BZX720855:BZX720878 CJT720855:CJT720878 CTP720855:CTP720878 DDL720855:DDL720878 DNH720855:DNH720878 DXD720855:DXD720878 EGZ720855:EGZ720878 EQV720855:EQV720878 FAR720855:FAR720878 FKN720855:FKN720878 FUJ720855:FUJ720878 GEF720855:GEF720878 GOB720855:GOB720878 GXX720855:GXX720878 HHT720855:HHT720878 HRP720855:HRP720878 IBL720855:IBL720878 ILH720855:ILH720878 IVD720855:IVD720878 JEZ720855:JEZ720878 JOV720855:JOV720878 JYR720855:JYR720878 KIN720855:KIN720878 KSJ720855:KSJ720878 LCF720855:LCF720878 LMB720855:LMB720878 LVX720855:LVX720878 MFT720855:MFT720878 MPP720855:MPP720878 MZL720855:MZL720878 NJH720855:NJH720878 NTD720855:NTD720878 OCZ720855:OCZ720878 OMV720855:OMV720878 OWR720855:OWR720878 PGN720855:PGN720878 PQJ720855:PQJ720878 QAF720855:QAF720878 QKB720855:QKB720878 QTX720855:QTX720878 RDT720855:RDT720878 RNP720855:RNP720878 RXL720855:RXL720878 SHH720855:SHH720878 SRD720855:SRD720878 TAZ720855:TAZ720878 TKV720855:TKV720878 TUR720855:TUR720878 UEN720855:UEN720878 UOJ720855:UOJ720878 UYF720855:UYF720878 VIB720855:VIB720878 VRX720855:VRX720878 WBT720855:WBT720878 WLP720855:WLP720878 WVL720855:WVL720878 C786392:C786415 IZ786391:IZ786414 SV786391:SV786414 ACR786391:ACR786414 AMN786391:AMN786414 AWJ786391:AWJ786414 BGF786391:BGF786414 BQB786391:BQB786414 BZX786391:BZX786414 CJT786391:CJT786414 CTP786391:CTP786414 DDL786391:DDL786414 DNH786391:DNH786414 DXD786391:DXD786414 EGZ786391:EGZ786414 EQV786391:EQV786414 FAR786391:FAR786414 FKN786391:FKN786414 FUJ786391:FUJ786414 GEF786391:GEF786414 GOB786391:GOB786414 GXX786391:GXX786414 HHT786391:HHT786414 HRP786391:HRP786414 IBL786391:IBL786414 ILH786391:ILH786414 IVD786391:IVD786414 JEZ786391:JEZ786414 JOV786391:JOV786414 JYR786391:JYR786414 KIN786391:KIN786414 KSJ786391:KSJ786414 LCF786391:LCF786414 LMB786391:LMB786414 LVX786391:LVX786414 MFT786391:MFT786414 MPP786391:MPP786414 MZL786391:MZL786414 NJH786391:NJH786414 NTD786391:NTD786414 OCZ786391:OCZ786414 OMV786391:OMV786414 OWR786391:OWR786414 PGN786391:PGN786414 PQJ786391:PQJ786414 QAF786391:QAF786414 QKB786391:QKB786414 QTX786391:QTX786414 RDT786391:RDT786414 RNP786391:RNP786414 RXL786391:RXL786414 SHH786391:SHH786414 SRD786391:SRD786414 TAZ786391:TAZ786414 TKV786391:TKV786414 TUR786391:TUR786414 UEN786391:UEN786414 UOJ786391:UOJ786414 UYF786391:UYF786414 VIB786391:VIB786414 VRX786391:VRX786414 WBT786391:WBT786414 WLP786391:WLP786414 WVL786391:WVL786414 C851928:C851951 IZ851927:IZ851950 SV851927:SV851950 ACR851927:ACR851950 AMN851927:AMN851950 AWJ851927:AWJ851950 BGF851927:BGF851950 BQB851927:BQB851950 BZX851927:BZX851950 CJT851927:CJT851950 CTP851927:CTP851950 DDL851927:DDL851950 DNH851927:DNH851950 DXD851927:DXD851950 EGZ851927:EGZ851950 EQV851927:EQV851950 FAR851927:FAR851950 FKN851927:FKN851950 FUJ851927:FUJ851950 GEF851927:GEF851950 GOB851927:GOB851950 GXX851927:GXX851950 HHT851927:HHT851950 HRP851927:HRP851950 IBL851927:IBL851950 ILH851927:ILH851950 IVD851927:IVD851950 JEZ851927:JEZ851950 JOV851927:JOV851950 JYR851927:JYR851950 KIN851927:KIN851950 KSJ851927:KSJ851950 LCF851927:LCF851950 LMB851927:LMB851950 LVX851927:LVX851950 MFT851927:MFT851950 MPP851927:MPP851950 MZL851927:MZL851950 NJH851927:NJH851950 NTD851927:NTD851950 OCZ851927:OCZ851950 OMV851927:OMV851950 OWR851927:OWR851950 PGN851927:PGN851950 PQJ851927:PQJ851950 QAF851927:QAF851950 QKB851927:QKB851950 QTX851927:QTX851950 RDT851927:RDT851950 RNP851927:RNP851950 RXL851927:RXL851950 SHH851927:SHH851950 SRD851927:SRD851950 TAZ851927:TAZ851950 TKV851927:TKV851950 TUR851927:TUR851950 UEN851927:UEN851950 UOJ851927:UOJ851950 UYF851927:UYF851950 VIB851927:VIB851950 VRX851927:VRX851950 WBT851927:WBT851950 WLP851927:WLP851950 WVL851927:WVL851950 C917464:C917487 IZ917463:IZ917486 SV917463:SV917486 ACR917463:ACR917486 AMN917463:AMN917486 AWJ917463:AWJ917486 BGF917463:BGF917486 BQB917463:BQB917486 BZX917463:BZX917486 CJT917463:CJT917486 CTP917463:CTP917486 DDL917463:DDL917486 DNH917463:DNH917486 DXD917463:DXD917486 EGZ917463:EGZ917486 EQV917463:EQV917486 FAR917463:FAR917486 FKN917463:FKN917486 FUJ917463:FUJ917486 GEF917463:GEF917486 GOB917463:GOB917486 GXX917463:GXX917486 HHT917463:HHT917486 HRP917463:HRP917486 IBL917463:IBL917486 ILH917463:ILH917486 IVD917463:IVD917486 JEZ917463:JEZ917486 JOV917463:JOV917486 JYR917463:JYR917486 KIN917463:KIN917486 KSJ917463:KSJ917486 LCF917463:LCF917486 LMB917463:LMB917486 LVX917463:LVX917486 MFT917463:MFT917486 MPP917463:MPP917486 MZL917463:MZL917486 NJH917463:NJH917486 NTD917463:NTD917486 OCZ917463:OCZ917486 OMV917463:OMV917486 OWR917463:OWR917486 PGN917463:PGN917486 PQJ917463:PQJ917486 QAF917463:QAF917486 QKB917463:QKB917486 QTX917463:QTX917486 RDT917463:RDT917486 RNP917463:RNP917486 RXL917463:RXL917486 SHH917463:SHH917486 SRD917463:SRD917486 TAZ917463:TAZ917486 TKV917463:TKV917486 TUR917463:TUR917486 UEN917463:UEN917486 UOJ917463:UOJ917486 UYF917463:UYF917486 VIB917463:VIB917486 VRX917463:VRX917486 WBT917463:WBT917486 WLP917463:WLP917486 WVL917463:WVL917486 C983000:C983023 IZ982999:IZ983022 SV982999:SV983022 ACR982999:ACR983022 AMN982999:AMN983022 AWJ982999:AWJ983022 BGF982999:BGF983022 BQB982999:BQB983022 BZX982999:BZX983022 CJT982999:CJT983022 CTP982999:CTP983022 DDL982999:DDL983022 DNH982999:DNH983022 DXD982999:DXD983022 EGZ982999:EGZ983022 EQV982999:EQV983022 FAR982999:FAR983022 FKN982999:FKN983022 FUJ982999:FUJ983022 GEF982999:GEF983022 GOB982999:GOB983022 GXX982999:GXX983022 HHT982999:HHT983022 HRP982999:HRP983022 IBL982999:IBL983022 ILH982999:ILH983022 IVD982999:IVD983022 JEZ982999:JEZ983022 JOV982999:JOV983022 JYR982999:JYR983022 KIN982999:KIN983022 KSJ982999:KSJ983022 LCF982999:LCF983022 LMB982999:LMB983022 LVX982999:LVX983022 MFT982999:MFT983022 MPP982999:MPP983022 MZL982999:MZL983022 NJH982999:NJH983022 NTD982999:NTD983022 OCZ982999:OCZ983022 OMV982999:OMV983022 OWR982999:OWR983022 PGN982999:PGN983022 PQJ982999:PQJ983022 QAF982999:QAF983022 QKB982999:QKB983022 QTX982999:QTX983022 RDT982999:RDT983022 RNP982999:RNP983022 RXL982999:RXL983022 SHH982999:SHH983022 SRD982999:SRD983022 TAZ982999:TAZ983022 TKV982999:TKV983022 TUR982999:TUR983022 UEN982999:UEN983022 UOJ982999:UOJ983022 UYF982999:UYF983022 VIB982999:VIB983022 VRX982999:VRX983022 WBT982999:WBT983022 WLP982999:WLP983022 WVL982999:WVL983022 D48:D51 SL25:SL29 WLF14:WLF23 WBJ14:WBJ23 VRN14:VRN23 VHR14:VHR23 UXV14:UXV23 UNZ14:UNZ23 UED14:UED23 TUH14:TUH23 TKL14:TKL23 TAP14:TAP23 SQT14:SQT23 SGX14:SGX23 RXB14:RXB23 RNF14:RNF23 RDJ14:RDJ23 QTN14:QTN23 QJR14:QJR23 PZV14:PZV23 PPZ14:PPZ23 PGD14:PGD23 OWH14:OWH23 OML14:OML23 OCP14:OCP23 NST14:NST23 NIX14:NIX23 MZB14:MZB23 MPF14:MPF23 MFJ14:MFJ23 LVN14:LVN23 LLR14:LLR23 LBV14:LBV23 KRZ14:KRZ23 KID14:KID23 JYH14:JYH23 JOL14:JOL23 JEP14:JEP23 IUT14:IUT23 IKX14:IKX23 IBB14:IBB23 HRF14:HRF23 HHJ14:HHJ23 GXN14:GXN23 GNR14:GNR23 GDV14:GDV23 FTZ14:FTZ23 FKD14:FKD23 FAH14:FAH23 EQL14:EQL23 EGP14:EGP23 DWT14:DWT23 DMX14:DMX23 DDB14:DDB23 CTF14:CTF23 CJJ14:CJJ23 BZN14:BZN23 BPR14:BPR23 BFV14:BFV23 AVZ14:AVZ23 AMD14:AMD23 ACH14:ACH23 SL14:SL23 IP14:IP23 WVB14:WVB23 WLG9:WLG13 WLQ6:WLQ8 WBK9:WBK13 WBU6:WBU8 VRO9:VRO13 VRY6:VRY8 VHS9:VHS13 VIC6:VIC8 UXW9:UXW13 UYG6:UYG8 UOA9:UOA13 UOK6:UOK8 UEE9:UEE13 UEO6:UEO8 TUI9:TUI13 TUS6:TUS8 TKM9:TKM13 TKW6:TKW8 TAQ9:TAQ13 TBA6:TBA8 SQU9:SQU13 SRE6:SRE8 SGY9:SGY13 SHI6:SHI8 RXC9:RXC13 RXM6:RXM8 RNG9:RNG13 RNQ6:RNQ8 RDK9:RDK13 RDU6:RDU8 QTO9:QTO13 QTY6:QTY8 QJS9:QJS13 QKC6:QKC8 PZW9:PZW13 QAG6:QAG8 PQA9:PQA13 PQK6:PQK8 PGE9:PGE13 PGO6:PGO8 OWI9:OWI13 OWS6:OWS8 OMM9:OMM13 OMW6:OMW8 OCQ9:OCQ13 ODA6:ODA8 NSU9:NSU13 NTE6:NTE8 NIY9:NIY13 NJI6:NJI8 MZC9:MZC13 MZM6:MZM8 MPG9:MPG13 MPQ6:MPQ8 MFK9:MFK13 MFU6:MFU8 LVO9:LVO13 LVY6:LVY8 LLS9:LLS13 LMC6:LMC8 LBW9:LBW13 LCG6:LCG8 KSA9:KSA13 KSK6:KSK8 KIE9:KIE13 KIO6:KIO8 JYI9:JYI13 JYS6:JYS8 JOM9:JOM13 JOW6:JOW8 JEQ9:JEQ13 JFA6:JFA8 IUU9:IUU13 IVE6:IVE8 IKY9:IKY13 ILI6:ILI8 IBC9:IBC13 IBM6:IBM8 HRG9:HRG13 HRQ6:HRQ8 HHK9:HHK13 HHU6:HHU8 GXO9:GXO13 GXY6:GXY8 GNS9:GNS13 GOC6:GOC8 GDW9:GDW13 GEG6:GEG8 FUA9:FUA13 FUK6:FUK8 FKE9:FKE13 FKO6:FKO8 FAI9:FAI13 FAS6:FAS8 EQM9:EQM13 EQW6:EQW8 EGQ9:EGQ13 EHA6:EHA8 DWU9:DWU13 DXE6:DXE8 DMY9:DMY13 DNI6:DNI8 DDC9:DDC13 DDM6:DDM8 CTG9:CTG13 CTQ6:CTQ8 CJK9:CJK13 CJU6:CJU8 BZO9:BZO13 BZY6:BZY8 BPS9:BPS13 BQC6:BQC8 BFW9:BFW13 BGG6:BGG8 AWA9:AWA13 AWK6:AWK8 AME9:AME13 AMO6:AMO8 ACI9:ACI13 ACS6:ACS8 SM9:SM13 SW6:SW8 IQ9:IQ13 JA6:JA8 WVC9:WVC13 WVM6:WVM8 D28:D29 SL33 IP33 WVB33 WLF33 WBJ33 VRN33 VHR33 UXV33 UNZ33 UED33 TUH33 TKL33 TAP33 SQT33 SGX33 RXB33 RNF33 RDJ33 QTN33 QJR33 PZV33 PPZ33 PGD33 OWH33 OML33 OCP33 NST33 NIX33 MZB33 MPF33 MFJ33 LVN33 LLR33 LBV33 KRZ33 KID33 JYH33 JOL33 JEP33 IUT33 IKX33 IBB33 HRF33 HHJ33 GXN33 GNR33 GDV33 FTZ33 FKD33 FAH33 EQL33 EGP33 DWT33 DMX33 DDB33 CTF33 CJJ33 BZN33 BPR33 BFV33 AVZ33 AMD33 ACH33 ABX30:ABX32 ACH25:ACH29 ALT30:ALT32 AMD25:AMD29 AVP30:AVP32 AVZ25:AVZ29 BFL30:BFL32 BFV25:BFV29 BPH30:BPH32 BPR25:BPR29 BZD30:BZD32 BZN25:BZN29 CIZ30:CIZ32 CJJ25:CJJ29 CSV30:CSV32 CTF25:CTF29 DCR30:DCR32 DDB25:DDB29 DMN30:DMN32 DMX25:DMX29 DWJ30:DWJ32 DWT25:DWT29 EGF30:EGF32 EGP25:EGP29 EQB30:EQB32 EQL25:EQL29 EZX30:EZX32 FAH25:FAH29 FJT30:FJT32 FKD25:FKD29 FTP30:FTP32 FTZ25:FTZ29 GDL30:GDL32 GDV25:GDV29 GNH30:GNH32 GNR25:GNR29 GXD30:GXD32 GXN25:GXN29 HGZ30:HGZ32 HHJ25:HHJ29 HQV30:HQV32 HRF25:HRF29 IAR30:IAR32 IBB25:IBB29 IKN30:IKN32 IKX25:IKX29 IUJ30:IUJ32 IUT25:IUT29 JEF30:JEF32 JEP25:JEP29 JOB30:JOB32 JOL25:JOL29 JXX30:JXX32 JYH25:JYH29 KHT30:KHT32 KID25:KID29 KRP30:KRP32 KRZ25:KRZ29 LBL30:LBL32 LBV25:LBV29 LLH30:LLH32 LLR25:LLR29 LVD30:LVD32 LVN25:LVN29 MEZ30:MEZ32 MFJ25:MFJ29 MOV30:MOV32 MPF25:MPF29 MYR30:MYR32 MZB25:MZB29 NIN30:NIN32 NIX25:NIX29 NSJ30:NSJ32 NST25:NST29 OCF30:OCF32 OCP25:OCP29 OMB30:OMB32 OML25:OML29 OVX30:OVX32 OWH25:OWH29 PFT30:PFT32 PGD25:PGD29 PPP30:PPP32 PPZ25:PPZ29 PZL30:PZL32 PZV25:PZV29 QJH30:QJH32 QJR25:QJR29 QTD30:QTD32 QTN25:QTN29 RCZ30:RCZ32 RDJ25:RDJ29 RMV30:RMV32 RNF25:RNF29 RWR30:RWR32 RXB25:RXB29 SGN30:SGN32 SGX25:SGX29 SQJ30:SQJ32 SQT25:SQT29 TAF30:TAF32 TAP25:TAP29 TKB30:TKB32 TKL25:TKL29 TTX30:TTX32 TUH25:TUH29 UDT30:UDT32 UED25:UED29 UNP30:UNP32 UNZ25:UNZ29 UXL30:UXL32 UXV25:UXV29 VHH30:VHH32 VHR25:VHR29 VRD30:VRD32 VRN25:VRN29 WAZ30:WAZ32 WBJ25:WBJ29 WKV30:WKV32 WLF25:WLF29 WUR30:WUR32 WVB25:WVB29 IF30:IF32 IP25:IP29 SB30:SB32 D134:D135 D100:D103 D6:D9 D55:D56 D64:D65 D73:D74 D82:D83 D126 D119:D120 D42:D43 D35:D36 D91:D92 D129 D22:D23 D108:D114 D13:D17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C65497:C65520 IZ65496:IZ65519 SV65496:SV65519 ACR65496:ACR65519 AMN65496:AMN65519 AWJ65496:AWJ65519 BGF65496:BGF65519 BQB65496:BQB65519 BZX65496:BZX65519 CJT65496:CJT65519 CTP65496:CTP65519 DDL65496:DDL65519 DNH65496:DNH65519 DXD65496:DXD65519 EGZ65496:EGZ65519 EQV65496:EQV65519 FAR65496:FAR65519 FKN65496:FKN65519 FUJ65496:FUJ65519 GEF65496:GEF65519 GOB65496:GOB65519 GXX65496:GXX65519 HHT65496:HHT65519 HRP65496:HRP65519 IBL65496:IBL65519 ILH65496:ILH65519 IVD65496:IVD65519 JEZ65496:JEZ65519 JOV65496:JOV65519 JYR65496:JYR65519 KIN65496:KIN65519 KSJ65496:KSJ65519 LCF65496:LCF65519 LMB65496:LMB65519 LVX65496:LVX65519 MFT65496:MFT65519 MPP65496:MPP65519 MZL65496:MZL65519 NJH65496:NJH65519 NTD65496:NTD65519 OCZ65496:OCZ65519 OMV65496:OMV65519 OWR65496:OWR65519 PGN65496:PGN65519 PQJ65496:PQJ65519 QAF65496:QAF65519 QKB65496:QKB65519 QTX65496:QTX65519 RDT65496:RDT65519 RNP65496:RNP65519 RXL65496:RXL65519 SHH65496:SHH65519 SRD65496:SRD65519 TAZ65496:TAZ65519 TKV65496:TKV65519 TUR65496:TUR65519 UEN65496:UEN65519 UOJ65496:UOJ65519 UYF65496:UYF65519 VIB65496:VIB65519 VRX65496:VRX65519 WBT65496:WBT65519 WLP65496:WLP65519 WVL65496:WVL65519 C131033:C131056 IZ131032:IZ131055 SV131032:SV131055 ACR131032:ACR131055 AMN131032:AMN131055 AWJ131032:AWJ131055 BGF131032:BGF131055 BQB131032:BQB131055 BZX131032:BZX131055 CJT131032:CJT131055 CTP131032:CTP131055 DDL131032:DDL131055 DNH131032:DNH131055 DXD131032:DXD131055 EGZ131032:EGZ131055 EQV131032:EQV131055 FAR131032:FAR131055 FKN131032:FKN131055 FUJ131032:FUJ131055 GEF131032:GEF131055 GOB131032:GOB131055 GXX131032:GXX131055 HHT131032:HHT131055 HRP131032:HRP131055 IBL131032:IBL131055 ILH131032:ILH131055 IVD131032:IVD131055 JEZ131032:JEZ131055 JOV131032:JOV131055 JYR131032:JYR131055 KIN131032:KIN131055 KSJ131032:KSJ131055 LCF131032:LCF131055 LMB131032:LMB131055 LVX131032:LVX131055 MFT131032:MFT131055 MPP131032:MPP131055 MZL131032:MZL131055 NJH131032:NJH131055 NTD131032:NTD131055 OCZ131032:OCZ131055 OMV131032:OMV131055 OWR131032:OWR131055 PGN131032:PGN131055 PQJ131032:PQJ131055 QAF131032:QAF131055 QKB131032:QKB131055 QTX131032:QTX131055 RDT131032:RDT131055 RNP131032:RNP131055 RXL131032:RXL131055 SHH131032:SHH131055 SRD131032:SRD131055 TAZ131032:TAZ131055 TKV131032:TKV131055 TUR131032:TUR131055 UEN131032:UEN131055 UOJ131032:UOJ131055 UYF131032:UYF131055 VIB131032:VIB131055 VRX131032:VRX131055 WBT131032:WBT131055 WLP131032:WLP131055 WVL131032:WVL131055 C196569:C196592 IZ196568:IZ196591 SV196568:SV196591 ACR196568:ACR196591 AMN196568:AMN196591 AWJ196568:AWJ196591 BGF196568:BGF196591 BQB196568:BQB196591 BZX196568:BZX196591 CJT196568:CJT196591 CTP196568:CTP196591 DDL196568:DDL196591 DNH196568:DNH196591 DXD196568:DXD196591 EGZ196568:EGZ196591 EQV196568:EQV196591 FAR196568:FAR196591 FKN196568:FKN196591 FUJ196568:FUJ196591 GEF196568:GEF196591 GOB196568:GOB196591 GXX196568:GXX196591 HHT196568:HHT196591 HRP196568:HRP196591 IBL196568:IBL196591 ILH196568:ILH196591 IVD196568:IVD196591 JEZ196568:JEZ196591 JOV196568:JOV196591 JYR196568:JYR196591 KIN196568:KIN196591 KSJ196568:KSJ196591 LCF196568:LCF196591 LMB196568:LMB196591 LVX196568:LVX196591 MFT196568:MFT196591 MPP196568:MPP196591 MZL196568:MZL196591 NJH196568:NJH196591 NTD196568:NTD196591 OCZ196568:OCZ196591 OMV196568:OMV196591 OWR196568:OWR196591 PGN196568:PGN196591 PQJ196568:PQJ196591 QAF196568:QAF196591 QKB196568:QKB196591 QTX196568:QTX196591 RDT196568:RDT196591 RNP196568:RNP196591 RXL196568:RXL196591 SHH196568:SHH196591 SRD196568:SRD196591 TAZ196568:TAZ196591 TKV196568:TKV196591 TUR196568:TUR196591 UEN196568:UEN196591 UOJ196568:UOJ196591 UYF196568:UYF196591 VIB196568:VIB196591 VRX196568:VRX196591 WBT196568:WBT196591 WLP196568:WLP196591 WVL196568:WVL196591 C262105:C262128 IZ262104:IZ262127 SV262104:SV262127 ACR262104:ACR262127 AMN262104:AMN262127 AWJ262104:AWJ262127 BGF262104:BGF262127 BQB262104:BQB262127 BZX262104:BZX262127 CJT262104:CJT262127 CTP262104:CTP262127 DDL262104:DDL262127 DNH262104:DNH262127 DXD262104:DXD262127 EGZ262104:EGZ262127 EQV262104:EQV262127 FAR262104:FAR262127 FKN262104:FKN262127 FUJ262104:FUJ262127 GEF262104:GEF262127 GOB262104:GOB262127 GXX262104:GXX262127 HHT262104:HHT262127 HRP262104:HRP262127 IBL262104:IBL262127 ILH262104:ILH262127 IVD262104:IVD262127 JEZ262104:JEZ262127 JOV262104:JOV262127 JYR262104:JYR262127 KIN262104:KIN262127 KSJ262104:KSJ262127 LCF262104:LCF262127 LMB262104:LMB262127 LVX262104:LVX262127 MFT262104:MFT262127 MPP262104:MPP262127 MZL262104:MZL262127 NJH262104:NJH262127 NTD262104:NTD262127 OCZ262104:OCZ262127 OMV262104:OMV262127 OWR262104:OWR262127 PGN262104:PGN262127 PQJ262104:PQJ262127 QAF262104:QAF262127 QKB262104:QKB262127 QTX262104:QTX262127 RDT262104:RDT262127 RNP262104:RNP262127 RXL262104:RXL262127 SHH262104:SHH262127 SRD262104:SRD262127 TAZ262104:TAZ262127 TKV262104:TKV262127 TUR262104:TUR262127 UEN262104:UEN262127 UOJ262104:UOJ262127 UYF262104:UYF262127 VIB262104:VIB262127 VRX262104:VRX262127 WBT262104:WBT262127 WLP262104:WLP262127 WVL262104:WVL262127 C327641:C327664 IZ327640:IZ327663 SV327640:SV327663 ACR327640:ACR327663 AMN327640:AMN327663 AWJ327640:AWJ327663 BGF327640:BGF327663 BQB327640:BQB327663 BZX327640:BZX327663 CJT327640:CJT327663 CTP327640:CTP327663 DDL327640:DDL327663 DNH327640:DNH327663 DXD327640:DXD327663 EGZ327640:EGZ327663 EQV327640:EQV327663 FAR327640:FAR327663 FKN327640:FKN327663 FUJ327640:FUJ327663 GEF327640:GEF327663 GOB327640:GOB327663 GXX327640:GXX327663 HHT327640:HHT327663 HRP327640:HRP327663 IBL327640:IBL327663 ILH327640:ILH327663 IVD327640:IVD327663 JEZ327640:JEZ327663 JOV327640:JOV327663 JYR327640:JYR327663 KIN327640:KIN327663 KSJ327640:KSJ327663 LCF327640:LCF327663 LMB327640:LMB327663 LVX327640:LVX327663 MFT327640:MFT327663 MPP327640:MPP327663 MZL327640:MZL327663 NJH327640:NJH327663 NTD327640:NTD327663 OCZ327640:OCZ327663 OMV327640:OMV327663 OWR327640:OWR327663 PGN327640:PGN327663 PQJ327640:PQJ327663 QAF327640:QAF327663 QKB327640:QKB327663 QTX327640:QTX327663 RDT327640:RDT327663 RNP327640:RNP327663 RXL327640:RXL327663 SHH327640:SHH327663 SRD327640:SRD327663 TAZ327640:TAZ327663 TKV327640:TKV327663 TUR327640:TUR327663 UEN327640:UEN327663 UOJ327640:UOJ327663 UYF327640:UYF327663 VIB327640:VIB327663 VRX327640:VRX327663 WBT327640:WBT327663 WLP327640:WLP327663 WVL327640:WVL327663 C393177:C393200 IZ393176:IZ393199 SV393176:SV393199 ACR393176:ACR393199 AMN393176:AMN393199 AWJ393176:AWJ393199 BGF393176:BGF393199 BQB393176:BQB393199 BZX393176:BZX393199 CJT393176:CJT393199 CTP393176:CTP393199 DDL393176:DDL393199 DNH393176:DNH393199 DXD393176:DXD393199 EGZ393176:EGZ393199 EQV393176:EQV393199 FAR393176:FAR393199 FKN393176:FKN393199 FUJ393176:FUJ393199 GEF393176:GEF393199 GOB393176:GOB393199 GXX393176:GXX393199 HHT393176:HHT393199 HRP393176:HRP393199 IBL393176:IBL393199 ILH393176:ILH393199 IVD393176:IVD393199 JEZ393176:JEZ393199 JOV393176:JOV393199 JYR393176:JYR393199 KIN393176:KIN393199 KSJ393176:KSJ393199 LCF393176:LCF393199 LMB393176:LMB393199 LVX393176:LVX393199 MFT393176:MFT393199 MPP393176:MPP393199 MZL393176:MZL393199 NJH393176:NJH393199 NTD393176:NTD393199 OCZ393176:OCZ393199 OMV393176:OMV393199 OWR393176:OWR393199 PGN393176:PGN393199 PQJ393176:PQJ393199 QAF393176:QAF393199 QKB393176:QKB393199 QTX393176:QTX393199 RDT393176:RDT393199 RNP393176:RNP393199 RXL393176:RXL393199 SHH393176:SHH393199 SRD393176:SRD393199 TAZ393176:TAZ393199 TKV393176:TKV393199 TUR393176:TUR393199 UEN393176:UEN393199 UOJ393176:UOJ393199 UYF393176:UYF393199 VIB393176:VIB393199 VRX393176:VRX393199 WBT393176:WBT393199 WLP393176:WLP393199 WVL393176:WVL393199 C458713:C458736 IZ458712:IZ458735 SV458712:SV458735 ACR458712:ACR458735 AMN458712:AMN458735 AWJ458712:AWJ458735 BGF458712:BGF458735 BQB458712:BQB458735 BZX458712:BZX458735 CJT458712:CJT458735 CTP458712:CTP458735 DDL458712:DDL458735 DNH458712:DNH458735 DXD458712:DXD458735 EGZ458712:EGZ458735 EQV458712:EQV458735 FAR458712:FAR458735 FKN458712:FKN458735 FUJ458712:FUJ458735 GEF458712:GEF458735 GOB458712:GOB458735 GXX458712:GXX458735 HHT458712:HHT458735 HRP458712:HRP458735 IBL458712:IBL458735 ILH458712:ILH458735 IVD458712:IVD458735 JEZ458712:JEZ458735 JOV458712:JOV458735 JYR458712:JYR458735 KIN458712:KIN458735 KSJ458712:KSJ458735 LCF458712:LCF458735 LMB458712:LMB458735 LVX458712:LVX458735 MFT458712:MFT458735 MPP458712:MPP458735 MZL458712:MZL458735 NJH458712:NJH458735 NTD458712:NTD458735 OCZ458712:OCZ458735 OMV458712:OMV458735 OWR458712:OWR458735 PGN458712:PGN458735 PQJ458712:PQJ458735 QAF458712:QAF458735 QKB458712:QKB458735 QTX458712:QTX458735 RDT458712:RDT458735 RNP458712:RNP458735 RXL458712:RXL458735 SHH458712:SHH458735 SRD458712:SRD458735 TAZ458712:TAZ458735 TKV458712:TKV458735 TUR458712:TUR458735 UEN458712:UEN458735 UOJ458712:UOJ458735 UYF458712:UYF458735 VIB458712:VIB458735 VRX458712:VRX458735 WBT458712:WBT458735 WLP458712:WLP458735 WVL458712:WVL458735 C524249:C524272 IZ524248:IZ524271 SV524248:SV524271 ACR524248:ACR524271 AMN524248:AMN524271 AWJ524248:AWJ524271 BGF524248:BGF524271 BQB524248:BQB524271 BZX524248:BZX524271 CJT524248:CJT524271 CTP524248:CTP524271 DDL524248:DDL524271 DNH524248:DNH524271 DXD524248:DXD524271 EGZ524248:EGZ524271 EQV524248:EQV524271 FAR524248:FAR524271 FKN524248:FKN524271 FUJ524248:FUJ524271 GEF524248:GEF524271 GOB524248:GOB524271 GXX524248:GXX524271 HHT524248:HHT524271 HRP524248:HRP524271 IBL524248:IBL524271 ILH524248:ILH524271 IVD524248:IVD524271 JEZ524248:JEZ524271 JOV524248:JOV524271 JYR524248:JYR524271 KIN524248:KIN524271 KSJ524248:KSJ524271 LCF524248:LCF524271 LMB524248:LMB524271 LVX524248:LVX524271 MFT524248:MFT524271 MPP524248:MPP524271 MZL524248:MZL524271 NJH524248:NJH524271 NTD524248:NTD524271 OCZ524248:OCZ524271 OMV524248:OMV524271 OWR524248:OWR524271 PGN524248:PGN524271 PQJ524248:PQJ524271 QAF524248:QAF524271 QKB524248:QKB524271 QTX524248:QTX524271 RDT524248:RDT524271 RNP524248:RNP524271 RXL524248:RXL524271 SHH524248:SHH524271 SRD524248:SRD524271 TAZ524248:TAZ524271 TKV524248:TKV524271 TUR524248:TUR524271 UEN524248:UEN524271 UOJ524248:UOJ524271 UYF524248:UYF524271 VIB524248:VIB524271 VRX524248:VRX524271 WBT524248:WBT524271 WLP524248:WLP524271 WVL524248:WVL524271 C589785:C589808 IZ589784:IZ589807 SV589784:SV589807 ACR589784:ACR589807 AMN589784:AMN589807 AWJ589784:AWJ589807 BGF589784:BGF589807 BQB589784:BQB589807 BZX589784:BZX589807 CJT589784:CJT589807 CTP589784:CTP589807 DDL589784:DDL589807 DNH589784:DNH589807 DXD589784:DXD589807 EGZ589784:EGZ589807 EQV589784:EQV589807 FAR589784:FAR589807 FKN589784:FKN589807 FUJ589784:FUJ589807 GEF589784:GEF589807 GOB589784:GOB589807 GXX589784:GXX589807 HHT589784:HHT589807 HRP589784:HRP589807 IBL589784:IBL589807 ILH589784:ILH589807 IVD589784:IVD589807 JEZ589784:JEZ589807 JOV589784:JOV589807 JYR589784:JYR589807 KIN589784:KIN589807 KSJ589784:KSJ589807 LCF589784:LCF589807 LMB589784:LMB589807 LVX589784:LVX589807 MFT589784:MFT589807 MPP589784:MPP589807 MZL589784:MZL589807 NJH589784:NJH589807 NTD589784:NTD589807 OCZ589784:OCZ589807 OMV589784:OMV589807 OWR589784:OWR589807 PGN589784:PGN589807 PQJ589784:PQJ589807 QAF589784:QAF589807 QKB589784:QKB589807 QTX589784:QTX589807 RDT589784:RDT589807 RNP589784:RNP589807 RXL589784:RXL589807 SHH589784:SHH589807 SRD589784:SRD589807 TAZ589784:TAZ589807 TKV589784:TKV589807 TUR589784:TUR589807 UEN589784:UEN589807 UOJ589784:UOJ589807 UYF589784:UYF589807 VIB589784:VIB589807 VRX589784:VRX589807 WBT589784:WBT589807 WLP589784:WLP589807 WVL589784:WVL589807 C655321:C655344 IZ655320:IZ655343 SV655320:SV655343 ACR655320:ACR655343 AMN655320:AMN655343 AWJ655320:AWJ655343 BGF655320:BGF655343 BQB655320:BQB655343 BZX655320:BZX655343 CJT655320:CJT655343 CTP655320:CTP655343 DDL655320:DDL655343 DNH655320:DNH655343 DXD655320:DXD655343 EGZ655320:EGZ655343 EQV655320:EQV655343 FAR655320:FAR655343 FKN655320:FKN655343 FUJ655320:FUJ655343 GEF655320:GEF655343 GOB655320:GOB655343 GXX655320:GXX655343 HHT655320:HHT655343 HRP655320:HRP655343 IBL655320:IBL655343 ILH655320:ILH655343 IVD655320:IVD655343 JEZ655320:JEZ655343 JOV655320:JOV655343 JYR655320:JYR655343 KIN655320:KIN655343 KSJ655320:KSJ655343 LCF655320:LCF655343 LMB655320:LMB655343 LVX655320:LVX655343 MFT655320:MFT655343 MPP655320:MPP655343 MZL655320:MZL655343 NJH655320:NJH655343 NTD655320:NTD655343 OCZ655320:OCZ655343 OMV655320:OMV655343 OWR655320:OWR655343 PGN655320:PGN655343 PQJ655320:PQJ655343 QAF655320:QAF655343 QKB655320:QKB655343 QTX655320:QTX655343 RDT655320:RDT655343 RNP655320:RNP655343 RXL655320:RXL655343 SHH655320:SHH655343 SRD655320:SRD655343 TAZ655320:TAZ655343 TKV655320:TKV655343 TUR655320:TUR655343 UEN655320:UEN655343 UOJ655320:UOJ655343 UYF655320:UYF655343 VIB655320:VIB655343 VRX655320:VRX655343 WBT655320:WBT655343 WLP655320:WLP655343 WVL655320:WVL655343 C720857:C720880 IZ720856:IZ720879 SV720856:SV720879 ACR720856:ACR720879 AMN720856:AMN720879 AWJ720856:AWJ720879 BGF720856:BGF720879 BQB720856:BQB720879 BZX720856:BZX720879 CJT720856:CJT720879 CTP720856:CTP720879 DDL720856:DDL720879 DNH720856:DNH720879 DXD720856:DXD720879 EGZ720856:EGZ720879 EQV720856:EQV720879 FAR720856:FAR720879 FKN720856:FKN720879 FUJ720856:FUJ720879 GEF720856:GEF720879 GOB720856:GOB720879 GXX720856:GXX720879 HHT720856:HHT720879 HRP720856:HRP720879 IBL720856:IBL720879 ILH720856:ILH720879 IVD720856:IVD720879 JEZ720856:JEZ720879 JOV720856:JOV720879 JYR720856:JYR720879 KIN720856:KIN720879 KSJ720856:KSJ720879 LCF720856:LCF720879 LMB720856:LMB720879 LVX720856:LVX720879 MFT720856:MFT720879 MPP720856:MPP720879 MZL720856:MZL720879 NJH720856:NJH720879 NTD720856:NTD720879 OCZ720856:OCZ720879 OMV720856:OMV720879 OWR720856:OWR720879 PGN720856:PGN720879 PQJ720856:PQJ720879 QAF720856:QAF720879 QKB720856:QKB720879 QTX720856:QTX720879 RDT720856:RDT720879 RNP720856:RNP720879 RXL720856:RXL720879 SHH720856:SHH720879 SRD720856:SRD720879 TAZ720856:TAZ720879 TKV720856:TKV720879 TUR720856:TUR720879 UEN720856:UEN720879 UOJ720856:UOJ720879 UYF720856:UYF720879 VIB720856:VIB720879 VRX720856:VRX720879 WBT720856:WBT720879 WLP720856:WLP720879 WVL720856:WVL720879 C786393:C786416 IZ786392:IZ786415 SV786392:SV786415 ACR786392:ACR786415 AMN786392:AMN786415 AWJ786392:AWJ786415 BGF786392:BGF786415 BQB786392:BQB786415 BZX786392:BZX786415 CJT786392:CJT786415 CTP786392:CTP786415 DDL786392:DDL786415 DNH786392:DNH786415 DXD786392:DXD786415 EGZ786392:EGZ786415 EQV786392:EQV786415 FAR786392:FAR786415 FKN786392:FKN786415 FUJ786392:FUJ786415 GEF786392:GEF786415 GOB786392:GOB786415 GXX786392:GXX786415 HHT786392:HHT786415 HRP786392:HRP786415 IBL786392:IBL786415 ILH786392:ILH786415 IVD786392:IVD786415 JEZ786392:JEZ786415 JOV786392:JOV786415 JYR786392:JYR786415 KIN786392:KIN786415 KSJ786392:KSJ786415 LCF786392:LCF786415 LMB786392:LMB786415 LVX786392:LVX786415 MFT786392:MFT786415 MPP786392:MPP786415 MZL786392:MZL786415 NJH786392:NJH786415 NTD786392:NTD786415 OCZ786392:OCZ786415 OMV786392:OMV786415 OWR786392:OWR786415 PGN786392:PGN786415 PQJ786392:PQJ786415 QAF786392:QAF786415 QKB786392:QKB786415 QTX786392:QTX786415 RDT786392:RDT786415 RNP786392:RNP786415 RXL786392:RXL786415 SHH786392:SHH786415 SRD786392:SRD786415 TAZ786392:TAZ786415 TKV786392:TKV786415 TUR786392:TUR786415 UEN786392:UEN786415 UOJ786392:UOJ786415 UYF786392:UYF786415 VIB786392:VIB786415 VRX786392:VRX786415 WBT786392:WBT786415 WLP786392:WLP786415 WVL786392:WVL786415 C851929:C851952 IZ851928:IZ851951 SV851928:SV851951 ACR851928:ACR851951 AMN851928:AMN851951 AWJ851928:AWJ851951 BGF851928:BGF851951 BQB851928:BQB851951 BZX851928:BZX851951 CJT851928:CJT851951 CTP851928:CTP851951 DDL851928:DDL851951 DNH851928:DNH851951 DXD851928:DXD851951 EGZ851928:EGZ851951 EQV851928:EQV851951 FAR851928:FAR851951 FKN851928:FKN851951 FUJ851928:FUJ851951 GEF851928:GEF851951 GOB851928:GOB851951 GXX851928:GXX851951 HHT851928:HHT851951 HRP851928:HRP851951 IBL851928:IBL851951 ILH851928:ILH851951 IVD851928:IVD851951 JEZ851928:JEZ851951 JOV851928:JOV851951 JYR851928:JYR851951 KIN851928:KIN851951 KSJ851928:KSJ851951 LCF851928:LCF851951 LMB851928:LMB851951 LVX851928:LVX851951 MFT851928:MFT851951 MPP851928:MPP851951 MZL851928:MZL851951 NJH851928:NJH851951 NTD851928:NTD851951 OCZ851928:OCZ851951 OMV851928:OMV851951 OWR851928:OWR851951 PGN851928:PGN851951 PQJ851928:PQJ851951 QAF851928:QAF851951 QKB851928:QKB851951 QTX851928:QTX851951 RDT851928:RDT851951 RNP851928:RNP851951 RXL851928:RXL851951 SHH851928:SHH851951 SRD851928:SRD851951 TAZ851928:TAZ851951 TKV851928:TKV851951 TUR851928:TUR851951 UEN851928:UEN851951 UOJ851928:UOJ851951 UYF851928:UYF851951 VIB851928:VIB851951 VRX851928:VRX851951 WBT851928:WBT851951 WLP851928:WLP851951 WVL851928:WVL851951 C917465:C917488 IZ917464:IZ917487 SV917464:SV917487 ACR917464:ACR917487 AMN917464:AMN917487 AWJ917464:AWJ917487 BGF917464:BGF917487 BQB917464:BQB917487 BZX917464:BZX917487 CJT917464:CJT917487 CTP917464:CTP917487 DDL917464:DDL917487 DNH917464:DNH917487 DXD917464:DXD917487 EGZ917464:EGZ917487 EQV917464:EQV917487 FAR917464:FAR917487 FKN917464:FKN917487 FUJ917464:FUJ917487 GEF917464:GEF917487 GOB917464:GOB917487 GXX917464:GXX917487 HHT917464:HHT917487 HRP917464:HRP917487 IBL917464:IBL917487 ILH917464:ILH917487 IVD917464:IVD917487 JEZ917464:JEZ917487 JOV917464:JOV917487 JYR917464:JYR917487 KIN917464:KIN917487 KSJ917464:KSJ917487 LCF917464:LCF917487 LMB917464:LMB917487 LVX917464:LVX917487 MFT917464:MFT917487 MPP917464:MPP917487 MZL917464:MZL917487 NJH917464:NJH917487 NTD917464:NTD917487 OCZ917464:OCZ917487 OMV917464:OMV917487 OWR917464:OWR917487 PGN917464:PGN917487 PQJ917464:PQJ917487 QAF917464:QAF917487 QKB917464:QKB917487 QTX917464:QTX917487 RDT917464:RDT917487 RNP917464:RNP917487 RXL917464:RXL917487 SHH917464:SHH917487 SRD917464:SRD917487 TAZ917464:TAZ917487 TKV917464:TKV917487 TUR917464:TUR917487 UEN917464:UEN917487 UOJ917464:UOJ917487 UYF917464:UYF917487 VIB917464:VIB917487 VRX917464:VRX917487 WBT917464:WBT917487 WLP917464:WLP917487 WVL917464:WVL917487 C983001:C983024 IZ983000:IZ983023 SV983000:SV983023 ACR983000:ACR983023 AMN983000:AMN983023 AWJ983000:AWJ983023 BGF983000:BGF983023 BQB983000:BQB983023 BZX983000:BZX983023 CJT983000:CJT983023 CTP983000:CTP983023 DDL983000:DDL983023 DNH983000:DNH983023 DXD983000:DXD983023 EGZ983000:EGZ983023 EQV983000:EQV983023 FAR983000:FAR983023 FKN983000:FKN983023 FUJ983000:FUJ983023 GEF983000:GEF983023 GOB983000:GOB983023 GXX983000:GXX983023 HHT983000:HHT983023 HRP983000:HRP983023 IBL983000:IBL983023 ILH983000:ILH983023 IVD983000:IVD983023 JEZ983000:JEZ983023 JOV983000:JOV983023 JYR983000:JYR983023 KIN983000:KIN983023 KSJ983000:KSJ983023 LCF983000:LCF983023 LMB983000:LMB983023 LVX983000:LVX983023 MFT983000:MFT983023 MPP983000:MPP983023 MZL983000:MZL983023 NJH983000:NJH983023 NTD983000:NTD983023 OCZ983000:OCZ983023 OMV983000:OMV983023 OWR983000:OWR983023 PGN983000:PGN983023 PQJ983000:PQJ983023 QAF983000:QAF983023 QKB983000:QKB983023 QTX983000:QTX983023 RDT983000:RDT983023 RNP983000:RNP983023 RXL983000:RXL983023 SHH983000:SHH983023 SRD983000:SRD983023 TAZ983000:TAZ983023 TKV983000:TKV983023 TUR983000:TUR983023 UEN983000:UEN983023 UOJ983000:UOJ983023 UYF983000:UYF983023 VIB983000:VIB983023 VRX983000:VRX983023 WBT983000:WBT983023 WLP983000:WLP983023 WVL983000:WVL983023 D48:D51 SL25:SL29 WLF14:WLF23 WBJ14:WBJ23 VRN14:VRN23 VHR14:VHR23 UXV14:UXV23 UNZ14:UNZ23 UED14:UED23 TUH14:TUH23 TKL14:TKL23 TAP14:TAP23 SQT14:SQT23 SGX14:SGX23 RXB14:RXB23 RNF14:RNF23 RDJ14:RDJ23 QTN14:QTN23 QJR14:QJR23 PZV14:PZV23 PPZ14:PPZ23 PGD14:PGD23 OWH14:OWH23 OML14:OML23 OCP14:OCP23 NST14:NST23 NIX14:NIX23 MZB14:MZB23 MPF14:MPF23 MFJ14:MFJ23 LVN14:LVN23 LLR14:LLR23 LBV14:LBV23 KRZ14:KRZ23 KID14:KID23 JYH14:JYH23 JOL14:JOL23 JEP14:JEP23 IUT14:IUT23 IKX14:IKX23 IBB14:IBB23 HRF14:HRF23 HHJ14:HHJ23 GXN14:GXN23 GNR14:GNR23 GDV14:GDV23 FTZ14:FTZ23 FKD14:FKD23 FAH14:FAH23 EQL14:EQL23 EGP14:EGP23 DWT14:DWT23 DMX14:DMX23 DDB14:DDB23 CTF14:CTF23 CJJ14:CJJ23 BZN14:BZN23 BPR14:BPR23 BFV14:BFV23 AVZ14:AVZ23 AMD14:AMD23 ACH14:ACH23 SL14:SL23 IP14:IP23 WVB14:WVB23 WLG9:WLG13 WLQ6:WLQ8 WBK9:WBK13 WBU6:WBU8 VRO9:VRO13 VRY6:VRY8 VHS9:VHS13 VIC6:VIC8 UXW9:UXW13 UYG6:UYG8 UOA9:UOA13 UOK6:UOK8 UEE9:UEE13 UEO6:UEO8 TUI9:TUI13 TUS6:TUS8 TKM9:TKM13 TKW6:TKW8 TAQ9:TAQ13 TBA6:TBA8 SQU9:SQU13 SRE6:SRE8 SGY9:SGY13 SHI6:SHI8 RXC9:RXC13 RXM6:RXM8 RNG9:RNG13 RNQ6:RNQ8 RDK9:RDK13 RDU6:RDU8 QTO9:QTO13 QTY6:QTY8 QJS9:QJS13 QKC6:QKC8 PZW9:PZW13 QAG6:QAG8 PQA9:PQA13 PQK6:PQK8 PGE9:PGE13 PGO6:PGO8 OWI9:OWI13 OWS6:OWS8 OMM9:OMM13 OMW6:OMW8 OCQ9:OCQ13 ODA6:ODA8 NSU9:NSU13 NTE6:NTE8 NIY9:NIY13 NJI6:NJI8 MZC9:MZC13 MZM6:MZM8 MPG9:MPG13 MPQ6:MPQ8 MFK9:MFK13 MFU6:MFU8 LVO9:LVO13 LVY6:LVY8 LLS9:LLS13 LMC6:LMC8 LBW9:LBW13 LCG6:LCG8 KSA9:KSA13 KSK6:KSK8 KIE9:KIE13 KIO6:KIO8 JYI9:JYI13 JYS6:JYS8 JOM9:JOM13 JOW6:JOW8 JEQ9:JEQ13 JFA6:JFA8 IUU9:IUU13 IVE6:IVE8 IKY9:IKY13 ILI6:ILI8 IBC9:IBC13 IBM6:IBM8 HRG9:HRG13 HRQ6:HRQ8 HHK9:HHK13 HHU6:HHU8 GXO9:GXO13 GXY6:GXY8 GNS9:GNS13 GOC6:GOC8 GDW9:GDW13 GEG6:GEG8 FUA9:FUA13 FUK6:FUK8 FKE9:FKE13 FKO6:FKO8 FAI9:FAI13 FAS6:FAS8 EQM9:EQM13 EQW6:EQW8 EGQ9:EGQ13 EHA6:EHA8 DWU9:DWU13 DXE6:DXE8 DMY9:DMY13 DNI6:DNI8 DDC9:DDC13 DDM6:DDM8 CTG9:CTG13 CTQ6:CTQ8 CJK9:CJK13 CJU6:CJU8 BZO9:BZO13 BZY6:BZY8 BPS9:BPS13 BQC6:BQC8 BFW9:BFW13 BGG6:BGG8 AWA9:AWA13 AWK6:AWK8 AME9:AME13 AMO6:AMO8 ACI9:ACI13 ACS6:ACS8 SM9:SM13 SW6:SW8 IQ9:IQ13 JA6:JA8 WVC9:WVC13 WVM6:WVM8 D28:D29 SL33 IP33 WVB33 WLF33 WBJ33 VRN33 VHR33 UXV33 UNZ33 UED33 TUH33 TKL33 TAP33 SQT33 SGX33 RXB33 RNF33 RDJ33 QTN33 QJR33 PZV33 PPZ33 PGD33 OWH33 OML33 OCP33 NST33 NIX33 MZB33 MPF33 MFJ33 LVN33 LLR33 LBV33 KRZ33 KID33 JYH33 JOL33 JEP33 IUT33 IKX33 IBB33 HRF33 HHJ33 GXN33 GNR33 GDV33 FTZ33 FKD33 FAH33 EQL33 EGP33 DWT33 DMX33 DDB33 CTF33 CJJ33 BZN33 BPR33 BFV33 AVZ33 AMD33 ACH33 ABX30:ABX32 ACH25:ACH29 ALT30:ALT32 AMD25:AMD29 AVP30:AVP32 AVZ25:AVZ29 BFL30:BFL32 BFV25:BFV29 BPH30:BPH32 BPR25:BPR29 BZD30:BZD32 BZN25:BZN29 CIZ30:CIZ32 CJJ25:CJJ29 CSV30:CSV32 CTF25:CTF29 DCR30:DCR32 DDB25:DDB29 DMN30:DMN32 DMX25:DMX29 DWJ30:DWJ32 DWT25:DWT29 EGF30:EGF32 EGP25:EGP29 EQB30:EQB32 EQL25:EQL29 EZX30:EZX32 FAH25:FAH29 FJT30:FJT32 FKD25:FKD29 FTP30:FTP32 FTZ25:FTZ29 GDL30:GDL32 GDV25:GDV29 GNH30:GNH32 GNR25:GNR29 GXD30:GXD32 GXN25:GXN29 HGZ30:HGZ32 HHJ25:HHJ29 HQV30:HQV32 HRF25:HRF29 IAR30:IAR32 IBB25:IBB29 IKN30:IKN32 IKX25:IKX29 IUJ30:IUJ32 IUT25:IUT29 JEF30:JEF32 JEP25:JEP29 JOB30:JOB32 JOL25:JOL29 JXX30:JXX32 JYH25:JYH29 KHT30:KHT32 KID25:KID29 KRP30:KRP32 KRZ25:KRZ29 LBL30:LBL32 LBV25:LBV29 LLH30:LLH32 LLR25:LLR29 LVD30:LVD32 LVN25:LVN29 MEZ30:MEZ32 MFJ25:MFJ29 MOV30:MOV32 MPF25:MPF29 MYR30:MYR32 MZB25:MZB29 NIN30:NIN32 NIX25:NIX29 NSJ30:NSJ32 NST25:NST29 OCF30:OCF32 OCP25:OCP29 OMB30:OMB32 OML25:OML29 OVX30:OVX32 OWH25:OWH29 PFT30:PFT32 PGD25:PGD29 PPP30:PPP32 PPZ25:PPZ29 PZL30:PZL32 PZV25:PZV29 QJH30:QJH32 QJR25:QJR29 QTD30:QTD32 QTN25:QTN29 RCZ30:RCZ32 RDJ25:RDJ29 RMV30:RMV32 RNF25:RNF29 RWR30:RWR32 RXB25:RXB29 SGN30:SGN32 SGX25:SGX29 SQJ30:SQJ32 SQT25:SQT29 TAF30:TAF32 TAP25:TAP29 TKB30:TKB32 TKL25:TKL29 TTX30:TTX32 TUH25:TUH29 UDT30:UDT32 UED25:UED29 UNP30:UNP32 UNZ25:UNZ29 UXL30:UXL32 UXV25:UXV29 VHH30:VHH32 VHR25:VHR29 VRD30:VRD32 VRN25:VRN29 WAZ30:WAZ32 WBJ25:WBJ29 WKV30:WKV32 WLF25:WLF29 WUR30:WUR32 WVB25:WVB29 IF30:IF32 IP25:IP29 SB30:SB32 D135:D136 D100:D103 D6:D9 D55:D56 D64:D65 D73:D74 D82:D83 D126 D119:D120 D42:D43 D35:D36 D91:D92 D129:D130 D22:D23 D108:D114 D13:D17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C19EFFB3EAC23140A73490829C1CC8B8" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac5988d82ddac3ab003e9d7bf87723ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3fb1b16c-9f7f-48ef-b0cb-65d9c2406ef1" xmlns:ns4="b15f7a1a-21a1-43a3-94c9-0b0dcb7d30b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4de3b7b99fa765833f05630728655cc0" ns3:_="" ns4:_="">
     <xsd:import namespace="3fb1b16c-9f7f-48ef-b0cb-65d9c2406ef1"/>
@@ -4527,24 +4574,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F5E1AF-B032-471F-8F72-CABBF98469E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C752205-2C46-4583-B75F-39719ECA802A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A54982A7-883B-4FD0-8F4E-87121E512EF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4561,4 +4606,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F5E1AF-B032-471F-8F72-CABBF98469E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C752205-2C46-4583-B75F-39719ECA802A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>